<commit_message>
updated Hospital Stay Mapping
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91AB00C-3717-4E8E-B908-F1F69B05D0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD4BE03-5D13-4A58-8EB0-51B0226D0912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="1" activeTab="4" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="IG-groups" sheetId="31" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="1311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="1347">
   <si>
     <t>Group Source</t>
   </si>
@@ -3678,15 +3678,6 @@
     <t>Preferred mapping</t>
   </si>
   <si>
-    <t>MedicationRequest.dosageInstruction</t>
-  </si>
-  <si>
-    <t>MedicationRequest.dosageInstruction.route</t>
-  </si>
-  <si>
-    <t>MedicationRequest.dosageInstruction.timing.repeat.duration</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHECK it is used the name period but the imression is that is the duration not the period </t>
   </si>
   <si>
@@ -3724,15 +3715,6 @@
   </si>
   <si>
     <t>MedicationDispense.daysSupply</t>
-  </si>
-  <si>
-    <t>MedicationDispense.dosageInstruction</t>
-  </si>
-  <si>
-    <t>MedicationDispense.dosageInstruction.route</t>
-  </si>
-  <si>
-    <t>MedicationDispense.dosageInstruction.timing.repeat.duration</t>
   </si>
   <si>
     <t>body.recommendations.carePlan</t>
@@ -4036,6 +4018,132 @@
   </si>
   <si>
     <t xml:space="preserve">Procedure.perfomedDateTime	</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/device-eu-hdr</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement.text</t>
+  </si>
+  <si>
+    <t>if referring to the description of the usage of the device</t>
+  </si>
+  <si>
+    <t>Device.text</t>
+  </si>
+  <si>
+    <t>if referring to the description of the device</t>
+  </si>
+  <si>
+    <t>Device.identifier</t>
+  </si>
+  <si>
+    <t>Details in the Composition.section:sectionMedicalDevices.entry of type DeviceUseStatement. See dedicated groups</t>
+  </si>
+  <si>
+    <t>if generic identifier</t>
+  </si>
+  <si>
+    <t>Device.udiCarrier</t>
+  </si>
+  <si>
+    <t>if it is the udiCarrier</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement.timing[x]</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement.timingPeriod.end</t>
+  </si>
+  <si>
+    <t>Procedure.perfomed[x]</t>
+  </si>
+  <si>
+    <t>If the usage period is highlighted</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/deviceUseStatement-eu-hdr</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement.reasonCode</t>
+  </si>
+  <si>
+    <t>DeviceUseStatement.reasonReference</t>
+  </si>
+  <si>
+    <t>if the implantation procedure is described</t>
+  </si>
+  <si>
+    <t>Details in the Composition.section:sectionMedications.entry. See dedicated groups</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.medicationCodeableConcept</t>
+  </si>
+  <si>
+    <t>MedicationStatement.medicationCodeableConcept</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Dosage</t>
+  </si>
+  <si>
+    <t>Dosage.route</t>
+  </si>
+  <si>
+    <t>Dosage.timing.repeat.duration</t>
+  </si>
+  <si>
+    <t>MedicationDispense.dosageInstruction or MedicationRequest.dosageInstruction or MedicationStatement.dosage</t>
+  </si>
+  <si>
+    <t>Dosage</t>
+  </si>
+  <si>
+    <t>MedicationAdministration</t>
+  </si>
+  <si>
+    <t>several elements used</t>
+  </si>
+  <si>
+    <t>MedicationStatement.effectivePeriod</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.occurencePeriod</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.dosage.route</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/MedicationAdministration</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/MedicationStatement</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.reasonCode</t>
+  </si>
+  <si>
+    <t>MedicationAdministration.reasonReference</t>
+  </si>
+  <si>
+    <t>MedicationRequest.reasonCode</t>
+  </si>
+  <si>
+    <t>MedicationRequest.reasonReference</t>
+  </si>
+  <si>
+    <t>MedicationDispense.reasonCode</t>
+  </si>
+  <si>
+    <t>MedicationDispense.reasonReference</t>
+  </si>
+  <si>
+    <t>MedicationStatement.reasonReference</t>
+  </si>
+  <si>
+    <t>MedicationStatement.reasonCode</t>
+  </si>
+  <si>
+    <t>MedicationRequest.dosageInstruction or MedicationDispense.dosageInstruction</t>
   </si>
 </sst>
 </file>
@@ -4110,7 +4218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -4157,6 +4265,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4166,7 +4296,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4209,7 +4339,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -4821,7 +4961,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>83</v>
@@ -4838,7 +4978,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>83</v>
@@ -4855,7 +4995,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>83</v>
@@ -4872,7 +5012,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>85</v>
@@ -4897,9 +5037,11 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -4962,8 +5104,8 @@
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>1212</v>
+      <c r="H2" s="9" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
@@ -4989,6 +5131,7 @@
       <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="str">
@@ -5013,14 +5156,17 @@
       <c r="G4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>1197</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
+      </c>
       <c r="B5" s="8" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A4</f>
@@ -5031,18 +5177,21 @@
         <v>A.2.9.2.3 - Code</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="7" t="s">
         <v>1197</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
+      </c>
       <c r="B6" s="8" t="s">
         <v>1190</v>
       </c>
@@ -5061,7 +5210,7 @@
       <c r="G6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>1198</v>
       </c>
     </row>
@@ -5088,6 +5237,7 @@
       <c r="G7" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="8" t="str">
@@ -5139,6 +5289,7 @@
       <c r="G9" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="8" t="str">
@@ -5163,11 +5314,15 @@
       <c r="G10" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A11" s="8"/>
+      <c r="A11" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
+      </c>
       <c r="B11" s="8" t="s">
-        <v>1211</v>
+        <v>1326</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A9</f>
@@ -5178,15 +5333,23 @@
         <v>A.2.9.2.8 - Dosage Regimen</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1215</v>
+        <v>1330</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>1346</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
+      </c>
       <c r="B12" s="8" t="s">
-        <v>1211</v>
+        <v>1326</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A10</f>
@@ -5197,15 +5360,21 @@
         <v>A.2.9.2.9 - Route of administration</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>1216</v>
+        <v>1327</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A13" s="8"/>
+      <c r="A13" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
+      </c>
       <c r="B13" s="8" t="s">
-        <v>1211</v>
+        <v>1326</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A11</f>
@@ -5215,15 +5384,15 @@
         <f>MedicationSummaryHdrEhn!D11</f>
         <v>A.2.9.2.10 - Period of treatment</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>1217</v>
+      <c r="E13" s="7" t="s">
+        <v>1328</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>1202</v>
+      <c r="H13" s="13" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
@@ -5235,97 +5404,24 @@
         <v>1188</v>
       </c>
       <c r="C14" s="7" t="str">
-        <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A9</f>
-        <v>MedicationSummary.dosageRegimen</v>
-      </c>
-      <c r="D14" s="7" t="str">
-        <f>MedicationSummaryHdrEhn!D9</f>
-        <v>A.2.9.2.8 - Dosage Regimen</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>1199</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A15" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C15" s="7" t="str">
-        <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A10</f>
-        <v>MedicationSummary.route</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f>MedicationSummaryHdrEhn!D10</f>
-        <v>A.2.9.2.9 - Route of administration</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>1200</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A16" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C16" s="7" t="str">
-        <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A11</f>
-        <v>MedicationSummary.period</v>
-      </c>
-      <c r="D16" s="13" t="str">
-        <f>MedicationSummaryHdrEhn!D11</f>
-        <v>A.2.9.2.10 - Period of treatment</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>1201</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A17" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$15</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/MedicationSummary</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C17" s="7" t="str">
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A12</f>
         <v>MedicationSummary.daysSupplied</v>
       </c>
-      <c r="D17" s="13" t="str">
+      <c r="D14" s="13" t="str">
         <f>MedicationSummaryHdrEhn!D12</f>
         <v>A.2.9.2.11 - Days supplied</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>1214</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="13" t="s">
+      <c r="E14" s="13" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A18" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A15" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5333,12 +5429,11 @@
     <hyperlink ref="B5" r:id="rId2" xr:uid="{5E536E8F-22F8-4BBD-8A14-500630308A95}"/>
     <hyperlink ref="B7:B10" r:id="rId3" display="http://hl7.eu/fhir/hdr/StructureDefinition/medication-eu-hdr" xr:uid="{953546B6-F2C1-40ED-AFDE-17BD5CFB4BDA}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{336E94C6-ED7B-44F9-A5A9-826A1FA82CC0}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{256BF4D5-7FED-42CF-881E-966AA286D6F0}"/>
-    <hyperlink ref="B12" r:id="rId6" xr:uid="{9AC4DE15-8934-4B61-903B-BDACAEC4AC30}"/>
-    <hyperlink ref="B13" r:id="rId7" xr:uid="{0E8C015A-98EF-414A-9067-1D0C301B1A5E}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{9A61A77A-3B2E-4EDD-A9EB-421D6100337D}"/>
+    <hyperlink ref="B12:B13" r:id="rId6" display="http://hl7.org/fhir/StructureDefinition/Dosage" xr:uid="{8EA8C0BB-2D98-4F28-8641-84CBF6E2AFBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -8149,8 +8244,8 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8378,20 +8473,20 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="C8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/hdr/ConceptMap/planOfCare2FHIR-eu-hdr</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>861</v>
@@ -8409,20 +8504,20 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.eu/fhir/hdr/ConceptMap/medicationSummary2FHIR-eu-hdr</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>861</v>
@@ -8440,20 +8535,20 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="C10" s="8" t="str">
         <f t="shared" ref="C10" si="1">"http://hl7.eu/fhir/hdr/ConceptMap/"&amp;A10</f>
         <v>http://hl7.eu/fhir/hdr/ConceptMap/hospitalStay2FHIR-eu-hdr</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>861</v>
@@ -14480,7 +14575,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -14611,10 +14706,10 @@
         <v>875</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1225</v>
+        <v>1219</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1244</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.75">
@@ -14625,10 +14720,10 @@
         <v>874</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1226</v>
+        <v>1220</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.75">
@@ -14639,38 +14734,38 @@
         <v>872</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1227</v>
+        <v>1221</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1242</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" s="7" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1239</v>
+        <v>1233</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1231</v>
+        <v>1225</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13" s="7" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>1238</v>
+        <v>1232</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.75">
@@ -14681,10 +14776,10 @@
         <v>1151</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1228</v>
+        <v>1222</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.75">
@@ -14695,10 +14790,10 @@
         <v>1152</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1229</v>
+        <v>1223</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1241</v>
+        <v>1235</v>
       </c>
     </row>
   </sheetData>
@@ -14727,10 +14822,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -14742,7 +14837,7 @@
     <col min="5" max="5" width="42.90625" customWidth="1"/>
     <col min="6" max="6" width="15.58984375" customWidth="1"/>
     <col min="7" max="7" width="11.1328125" customWidth="1"/>
-    <col min="8" max="8" width="64.7265625" customWidth="1"/>
+    <col min="8" max="8" width="64.7265625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.75">
@@ -14767,11 +14862,11 @@
       <c r="G1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
@@ -14788,14 +14883,14 @@
         <v>HospitalStay.A.2.7.1 - Diagnostic summary</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>1277</v>
+      <c r="H2" s="9" t="s">
+        <v>1271</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
@@ -14804,7 +14899,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C3" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A3</f>
@@ -14815,7 +14910,7 @@
         <v>HospitalStay.A.2.7.1.1 - Problem description</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7" t="s">
@@ -14829,7 +14924,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C4" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A4</f>
@@ -14840,7 +14935,7 @@
         <v>HospitalStay.A.2.7.1.2 - Problem details</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
@@ -14854,7 +14949,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C5" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A5</f>
@@ -14865,7 +14960,7 @@
         <v>HospitalStay.A.2.7.1.3 - Onset date</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
@@ -14879,7 +14974,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C6" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A6</f>
@@ -14890,7 +14985,7 @@
         <v>HospitalStay.A.2.7.1.4 - End date</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
@@ -14904,7 +14999,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C7" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A7</f>
@@ -14915,7 +15010,7 @@
         <v>HospitalStay.A.2.7.1.5 - Category</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
@@ -14929,7 +15024,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C8" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A8</f>
@@ -14940,7 +15035,7 @@
         <v>HospitalStay.A.2.7.1.6 - Treatment class</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
@@ -14954,7 +15049,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C9" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A9</f>
@@ -14965,7 +15060,7 @@
         <v>HospitalStay.A.2.7.1.7 - Clinical status</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
@@ -14979,7 +15074,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C10" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A10</f>
@@ -14997,7 +15092,7 @@
         <v>22</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
@@ -15006,7 +15101,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C11" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A11</f>
@@ -15017,7 +15112,7 @@
         <v>HospitalStay.A.2.7.1.9 - Severity</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
@@ -15031,7 +15126,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="C12" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A12</f>
@@ -15042,7 +15137,7 @@
         <v>HospitalStay.A.2.7.1.10 - Stage</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
@@ -15050,7 +15145,7 @@
       </c>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A13" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
@@ -15067,14 +15162,14 @@
         <v>HospitalStay.A.2.7.2 - Significant procedures</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>1298</v>
+      <c r="H13" s="9" t="s">
+        <v>1292</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
@@ -15083,7 +15178,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C14" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A14</f>
@@ -15094,7 +15189,7 @@
         <v>HospitalStay.A.2.7.2.1 - Procedure code</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
@@ -15108,7 +15203,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C15" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A15</f>
@@ -15119,7 +15214,7 @@
         <v>HospitalStay.A.2.7.2.2 - Procedure description</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
@@ -15133,7 +15228,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C16" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A16</f>
@@ -15144,7 +15239,7 @@
         <v>HospitalStay.A.2.7.2.3 - Body site</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
@@ -15158,7 +15253,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C17" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A16</f>
@@ -15169,14 +15264,14 @@
         <v>HospitalStay.A.2.7.2.3 - Body site</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
@@ -15185,7 +15280,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C18" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A17</f>
@@ -15196,7 +15291,7 @@
         <v>HospitalStay.A.2.7.2.4 - Procedure date</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
@@ -15210,7 +15305,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C19" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A18</f>
@@ -15221,7 +15316,7 @@
         <v>HospitalStay.A.2.7.2.5 - Procedure reason</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7" t="s">
@@ -15230,12 +15325,12 @@
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A20" s="11" t="str">
+      <c r="A20" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C20" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A18</f>
@@ -15246,7 +15341,7 @@
         <v>HospitalStay.A.2.7.2.5 - Procedure reason</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
@@ -15255,12 +15350,12 @@
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A21" s="11" t="str">
+      <c r="A21" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C21" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A19</f>
@@ -15271,7 +15366,7 @@
         <v>HospitalStay.A.2.7.2.6 - Outcome</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -15280,12 +15375,12 @@
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A22" s="11" t="str">
+      <c r="A22" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C22" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A20</f>
@@ -15296,7 +15391,7 @@
         <v>HospitalStay.A.2.7.2.7 - Complication</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
@@ -15305,12 +15400,12 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A23" s="11" t="str">
+      <c r="A23" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C23" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A20</f>
@@ -15321,21 +15416,20 @@
         <v>HospitalStay.A.2.7.2.7 - Complication</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>1308</v>
-      </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="7" t="s">
+        <v>1302</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A24" s="11" t="str">
+      <c r="A24" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="C24" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A21</f>
@@ -15346,14 +15440,15 @@
         <v>HospitalStay.A.2.7.2.8 - Focal device</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>1309</v>
-      </c>
+        <v>1303</v>
+      </c>
+      <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A25" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
@@ -15370,11 +15465,14 @@
         <v>HospitalStay.A.2.7.3 - Medical devices and implants</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>1311</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
@@ -15383,7 +15481,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>902</v>
+        <v>1319</v>
       </c>
       <c r="C26" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A23</f>
@@ -15394,13 +15492,14 @@
         <v>HospitalStay.A.2.7.3.1 - Device and implant description</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G26" s="13" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>1287</v>
+      <c r="H26" s="9" t="s">
+        <v>1307</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
@@ -15409,24 +15508,25 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>902</v>
+        <v>1305</v>
       </c>
       <c r="C27" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A24</f>
-        <v>HospitalStay.medicalDevices.identifier</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A23</f>
+        <v>HospitalStay.medicalDevices.description</v>
       </c>
       <c r="D27" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D24</f>
-        <v>HospitalStay.A.2.7.3.2 - Device ID</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D23</f>
+        <v>HospitalStay.A.2.7.3.1 - Device and implant description</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G27" s="13" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="14" t="s">
-        <v>1287</v>
+      <c r="H27" s="9" t="s">
+        <v>1309</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
@@ -15435,24 +15535,25 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>902</v>
+        <v>1305</v>
       </c>
       <c r="C28" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A25</f>
-        <v>HospitalStay.medicalDevices.implantDate</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A24</f>
+        <v>HospitalStay.medicalDevices.identifier</v>
       </c>
       <c r="D28" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D25</f>
-        <v>HospitalStay.A.2.7.3.3 - Implant date</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D24</f>
+        <v>HospitalStay.A.2.7.3.2 - Device ID</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G28" s="13" t="s">
+        <v>1310</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="14" t="s">
-        <v>1287</v>
+      <c r="H28" s="9" t="s">
+        <v>1312</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
@@ -15461,24 +15562,25 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>902</v>
+        <v>1305</v>
       </c>
       <c r="C29" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A26</f>
-        <v>HospitalStay.medicalDevices.endDate</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A24</f>
+        <v>HospitalStay.medicalDevices.identifier</v>
       </c>
       <c r="D29" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D26</f>
-        <v>HospitalStay.A.2.7.3.4 - End date</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D24</f>
+        <v>HospitalStay.A.2.7.3.2 - Device ID</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G29" s="13" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="14" t="s">
-        <v>1287</v>
+      <c r="H29" s="9" t="s">
+        <v>1314</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
@@ -15487,24 +15589,25 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>902</v>
+        <v>1319</v>
       </c>
       <c r="C30" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A27</f>
-        <v>HospitalStay.medicalDevices.reason</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A25</f>
+        <v>HospitalStay.medicalDevices.implantDate</v>
       </c>
       <c r="D30" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D27</f>
-        <v>HospitalStay.A.2.7.3.5 - Reason</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D25</f>
+        <v>HospitalStay.A.2.7.3.3 - Implant date</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>1289</v>
-      </c>
-      <c r="G30" s="13" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="14" t="s">
-        <v>1287</v>
+      <c r="H30" s="9" t="s">
+        <v>1318</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
@@ -15513,23 +15616,26 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>902</v>
+        <v>1291</v>
       </c>
       <c r="C31" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A28</f>
-        <v>HospitalStay.pharmacotherapy</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A25</f>
+        <v>HospitalStay.medicalDevices.implantDate</v>
       </c>
       <c r="D31" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D28</f>
-        <v>HospitalStay.A.2.7.5 - Pharmacotherapy</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D25</f>
+        <v>HospitalStay.A.2.7.3.3 - Implant date</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G31" s="13" t="s">
+        <v>1317</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="15"/>
+      <c r="H31" s="9" t="s">
+        <v>1322</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="8" t="str">
@@ -15537,25 +15643,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>902</v>
+        <v>1319</v>
       </c>
       <c r="C32" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
-        <v>HospitalStay.pharmacotherapy.reason</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A26</f>
+        <v>HospitalStay.medicalDevices.endDate</v>
       </c>
       <c r="D32" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
-        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D26</f>
+        <v>HospitalStay.A.2.7.3.4 - End date</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G32" s="13" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="14" t="s">
-        <v>1287</v>
-      </c>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A33" s="8" t="str">
@@ -15563,25 +15668,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>902</v>
+        <v>1319</v>
       </c>
       <c r="C33" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
-        <v>HospitalStay.pharmacotherapy.productCode</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A27</f>
+        <v>HospitalStay.medicalDevices.reason</v>
       </c>
       <c r="D33" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
-        <v>HospitalStay.A.2.7.5.2 - Code</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D27</f>
+        <v>HospitalStay.A.2.7.3.5 - Reason</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G33" s="13" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="14" t="s">
-        <v>1287</v>
-      </c>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="8" t="str">
@@ -15589,27 +15693,26 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>902</v>
+        <v>1319</v>
       </c>
       <c r="C34" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A31</f>
-        <v>HospitalStay.pharmacotherapy.intendedUse</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A27</f>
+        <v>HospitalStay.medicalDevices.reason</v>
       </c>
       <c r="D34" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D31</f>
-        <v>HospitalStay.A.2.7.5.3 - Intended use</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D27</f>
+        <v>HospitalStay.A.2.7.3.5 - Reason</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G34" s="13" t="s">
+        <v>1321</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="14" t="s">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A35" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
@@ -15618,21 +15721,22 @@
         <v>902</v>
       </c>
       <c r="C35" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A32</f>
-        <v>HospitalStay.pharmacotherapy.productName</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A28</f>
+        <v>HospitalStay.pharmacotherapy</v>
       </c>
       <c r="D35" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D32</f>
-        <v>HospitalStay.A.2.7.5.4 - Brand name</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D28</f>
+        <v>HospitalStay.A.2.7.5 - Pharmacotherapy</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>1290</v>
-      </c>
+        <v>1284</v>
+      </c>
+      <c r="F35" s="7"/>
       <c r="G35" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="14" t="s">
-        <v>1287</v>
+      <c r="H35" s="9" t="s">
+        <v>1323</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.75">
@@ -15641,25 +15745,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>902</v>
+        <v>1336</v>
       </c>
       <c r="C36" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A33</f>
-        <v>HospitalStay.pharmacotherapy.activeIngredient</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D36" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D33</f>
-        <v>HospitalStay.A.2.7.5.5 - Active ingredient list</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <v>1338</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A37" s="8" t="str">
@@ -15667,25 +15770,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>902</v>
+        <v>1336</v>
       </c>
       <c r="C37" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A34</f>
-        <v>HospitalStay.pharmacotherapy.strength</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D37" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D34</f>
-        <v>HospitalStay.A.2.7.5.6 - Strength</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <v>1339</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A38" s="8" t="str">
@@ -15693,25 +15795,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>902</v>
+        <v>1188</v>
       </c>
       <c r="C38" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A35</f>
-        <v>HospitalStay.pharmacotherapy.doseForm</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D38" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D35</f>
-        <v>HospitalStay.A.2.7.5.7 - Pharmaceutical dose form</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A39" s="8" t="str">
@@ -15719,25 +15820,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>902</v>
+        <v>1188</v>
       </c>
       <c r="C39" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A36</f>
-        <v>HospitalStay.pharmacotherapy.dosageRegimen</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D39" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D36</f>
-        <v>HospitalStay.A.2.7.5.8 - Dosage Regimen</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>1341</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A40" s="8" t="str">
@@ -15745,25 +15845,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>902</v>
+        <v>1208</v>
       </c>
       <c r="C40" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A37</f>
-        <v>HospitalStay.pharmacotherapy.route</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D40" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D37</f>
-        <v>HospitalStay.A.2.7.5.9 - Route of administration</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A41" s="8" t="str">
@@ -15771,25 +15870,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>902</v>
+        <v>1208</v>
       </c>
       <c r="C41" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A38</f>
-        <v>HospitalStay.pharmacotherapy.period</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D41" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D38</f>
-        <v>HospitalStay.A.2.7.5.10 - Period of treatment</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>1343</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A42" s="8" t="str">
@@ -15797,23 +15895,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>902</v>
+        <v>1337</v>
       </c>
       <c r="C42" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A39</f>
-        <v>HospitalStay.significantResults</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D42" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D39</f>
-        <v>HospitalStay.A.2.7.6 - Significant Observation Results</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="15"/>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A43" s="8" t="str">
@@ -15821,25 +15920,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>902</v>
+        <v>1337</v>
       </c>
       <c r="C43" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A40</f>
-        <v>HospitalStay.significantResults.date</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A29</f>
+        <v>HospitalStay.pharmacotherapy.reason</v>
       </c>
       <c r="D43" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D40</f>
-        <v>HospitalStay.A.2.7.6.1 - Date</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D29</f>
+        <v>HospitalStay.A.2.7.5.1 - Medication reason</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A44" s="8" t="str">
@@ -15847,25 +15945,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>902</v>
+        <v>1188</v>
       </c>
       <c r="C44" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A41</f>
-        <v>HospitalStay.significantResults.status</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
+        <v>HospitalStay.pharmacotherapy.productCode</v>
       </c>
       <c r="D44" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D41</f>
-        <v>HospitalStay.A.2.7.6.2 - Observation status</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
+        <v>HospitalStay.A.2.7.5.2 - Code</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A45" s="8" t="str">
@@ -15873,25 +15970,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>902</v>
+        <v>1208</v>
       </c>
       <c r="C45" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A42</f>
-        <v>HospitalStay.significantResults.description</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
+        <v>HospitalStay.pharmacotherapy.productCode</v>
       </c>
       <c r="D45" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D42</f>
-        <v>HospitalStay.A.2.7.6.3 - Result description</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
+        <v>HospitalStay.A.2.7.5.2 - Code</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A46" s="8" t="str">
@@ -15899,25 +15995,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>902</v>
+        <v>1336</v>
       </c>
       <c r="C46" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A43</f>
-        <v>HospitalStay.significantResults.details</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
+        <v>HospitalStay.pharmacotherapy.productCode</v>
       </c>
       <c r="D46" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D43</f>
-        <v>HospitalStay.A.2.7.6.4 - Observation details</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
+        <v>HospitalStay.A.2.7.5.2 - Code</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>1324</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A47" s="8" t="str">
@@ -15925,25 +16020,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>902</v>
+        <v>1337</v>
       </c>
       <c r="C47" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A44</f>
-        <v>HospitalStay.significantResults.result</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
+        <v>HospitalStay.pharmacotherapy.productCode</v>
       </c>
       <c r="D47" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D44</f>
-        <v>HospitalStay.A.2.7.6.5 - Observation result</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
+        <v>HospitalStay.A.2.7.5.2 - Code</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>1325</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A48" s="8" t="str">
@@ -15951,25 +16045,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>902</v>
+        <v>1190</v>
       </c>
       <c r="C48" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A45</f>
-        <v>HospitalStay.significantResults.reporter</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A30</f>
+        <v>HospitalStay.pharmacotherapy.productCode</v>
       </c>
       <c r="D48" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D45</f>
-        <v>HospitalStay.A.2.7.6.7 - Reporter</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>1291</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D30</f>
+        <v>HospitalStay.A.2.7.5.2 - Code</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A49" s="8" t="str">
@@ -15977,23 +16070,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>902</v>
+        <v>1190</v>
       </c>
       <c r="C49" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A46</f>
-        <v>HospitalStay.synthesis</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A31</f>
+        <v>HospitalStay.pharmacotherapy.intendedUse</v>
       </c>
       <c r="D49" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D46</f>
-        <v>HospitalStay.A.2.7.7 - Synthesis</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D31</f>
+        <v>HospitalStay.A.2.7.5.3 - Intended use</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>1292</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H49" s="15"/>
+        <v>1284</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A50" s="8" t="str">
@@ -16001,25 +16095,24 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>902</v>
+        <v>1190</v>
       </c>
       <c r="C50" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A47</f>
-        <v>HospitalStay.synthesis.description</v>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A32</f>
+        <v>HospitalStay.pharmacotherapy.productName</v>
       </c>
       <c r="D50" s="9" t="str">
-        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D47</f>
-        <v>HospitalStay.A.2.7.7.1 - Problem synthesis</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>1292</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>1287</v>
-      </c>
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D32</f>
+        <v>HospitalStay.A.2.7.5.4 - Brand name</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A51" s="8" t="str">
@@ -16027,25 +16120,598 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C51" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A33</f>
+        <v>HospitalStay.pharmacotherapy.activeIngredient</v>
+      </c>
+      <c r="D51" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D33</f>
+        <v>HospitalStay.A.2.7.5.5 - Active ingredient list</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A52" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C52" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A34</f>
+        <v>HospitalStay.pharmacotherapy.strength</v>
+      </c>
+      <c r="D52" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D34</f>
+        <v>HospitalStay.A.2.7.5.6 - Strength</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A53" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C53" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A35</f>
+        <v>HospitalStay.pharmacotherapy.doseForm</v>
+      </c>
+      <c r="D53" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D35</f>
+        <v>HospitalStay.A.2.7.5.7 - Pharmaceutical dose form</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A54" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C54" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A36</f>
+        <v>HospitalStay.pharmacotherapy.dosageRegimen</v>
+      </c>
+      <c r="D54" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D36</f>
+        <v>HospitalStay.A.2.7.5.8 - Dosage Regimen</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A55" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C55" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A36</f>
+        <v>HospitalStay.pharmacotherapy.dosageRegimen</v>
+      </c>
+      <c r="D55" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D36</f>
+        <v>HospitalStay.A.2.7.5.8 - Dosage Regimen</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1331</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A56" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C56" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A37</f>
+        <v>HospitalStay.pharmacotherapy.route</v>
+      </c>
+      <c r="D56" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D37</f>
+        <v>HospitalStay.A.2.7.5.9 - Route of administration</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A57" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C57" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A37</f>
+        <v>HospitalStay.pharmacotherapy.route</v>
+      </c>
+      <c r="D57" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D37</f>
+        <v>HospitalStay.A.2.7.5.9 - Route of administration</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1335</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A58" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C58" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A38</f>
+        <v>HospitalStay.pharmacotherapy.period</v>
+      </c>
+      <c r="D58" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D38</f>
+        <v>HospitalStay.A.2.7.5.10 - Period of treatment</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A59" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C59" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A38</f>
+        <v>HospitalStay.pharmacotherapy.period</v>
+      </c>
+      <c r="D59" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D38</f>
+        <v>HospitalStay.A.2.7.5.10 - Period of treatment</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1334</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A60" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C60" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A38</f>
+        <v>HospitalStay.pharmacotherapy.period</v>
+      </c>
+      <c r="D60" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D38</f>
+        <v>HospitalStay.A.2.7.5.10 - Period of treatment</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" s="25"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A61" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>902</v>
       </c>
-      <c r="C51" s="9" t="str">
+      <c r="C61" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A39</f>
+        <v>HospitalStay.significantResults</v>
+      </c>
+      <c r="D61" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D39</f>
+        <v>HospitalStay.A.2.7.6 - Significant Observation Results</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A62" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C62" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A40</f>
+        <v>HospitalStay.significantResults.date</v>
+      </c>
+      <c r="D62" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D40</f>
+        <v>HospitalStay.A.2.7.6.1 - Date</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A63" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C63" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A41</f>
+        <v>HospitalStay.significantResults.status</v>
+      </c>
+      <c r="D63" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D41</f>
+        <v>HospitalStay.A.2.7.6.2 - Observation status</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A64" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C64" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A42</f>
+        <v>HospitalStay.significantResults.description</v>
+      </c>
+      <c r="D64" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D42</f>
+        <v>HospitalStay.A.2.7.6.3 - Result description</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A65" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C65" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A43</f>
+        <v>HospitalStay.significantResults.details</v>
+      </c>
+      <c r="D65" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D43</f>
+        <v>HospitalStay.A.2.7.6.4 - Observation details</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A66" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C66" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A44</f>
+        <v>HospitalStay.significantResults.result</v>
+      </c>
+      <c r="D66" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D44</f>
+        <v>HospitalStay.A.2.7.6.5 - Observation result</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A67" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C67" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A45</f>
+        <v>HospitalStay.significantResults.reporter</v>
+      </c>
+      <c r="D67" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D45</f>
+        <v>HospitalStay.A.2.7.6.7 - Reporter</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A68" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C68" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A46</f>
+        <v>HospitalStay.synthesis</v>
+      </c>
+      <c r="D68" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D46</f>
+        <v>HospitalStay.A.2.7.7 - Synthesis</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="14"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A69" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C69" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A47</f>
+        <v>HospitalStay.synthesis.description</v>
+      </c>
+      <c r="D69" s="9" t="str">
+        <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D47</f>
+        <v>HospitalStay.A.2.7.7.1 - Problem synthesis</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A70" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>902</v>
+      </c>
+      <c r="C70" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A48</f>
         <v>HospitalStay.synthesis.reasoning</v>
       </c>
-      <c r="D51" s="9" t="str">
+      <c r="D70" s="9" t="str">
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!D48</f>
         <v>HospitalStay.A.2.7.7.2 - Clinical reasoning</v>
       </c>
-      <c r="E51" s="9" t="s">
-        <v>1292</v>
-      </c>
-      <c r="G51" s="13" t="s">
+      <c r="E70" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H51" s="14" t="s">
-        <v>1287</v>
-      </c>
+      <c r="H70" s="14" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="B73" s="8"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="B74" s="8"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="B75" s="8"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.75">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -16055,46 +16721,55 @@
     <hyperlink ref="B2" r:id="rId4" xr:uid="{9D31C99A-4131-437D-908C-E577823AA465}"/>
     <hyperlink ref="B13" r:id="rId5" xr:uid="{0608F21A-4822-44AC-8BD3-95B85DA34FF4}"/>
     <hyperlink ref="B26" r:id="rId6" xr:uid="{F7275174-C5B2-4943-8EDD-7C4D82FA0A08}"/>
-    <hyperlink ref="B28" r:id="rId7" xr:uid="{C77926B4-7EE1-4EC6-B4C5-0473052445EF}"/>
-    <hyperlink ref="B30" r:id="rId8" xr:uid="{48985362-312B-4345-874D-2EA3BF6DAA17}"/>
-    <hyperlink ref="B32" r:id="rId9" xr:uid="{87F54F97-6E1A-4607-86DD-1C7AEC637F46}"/>
-    <hyperlink ref="B34" r:id="rId10" xr:uid="{14F23EC8-0F33-4FEE-8B85-27AAA0415817}"/>
-    <hyperlink ref="B36" r:id="rId11" xr:uid="{7EC4BA8B-7C06-4590-B90B-ED095D98CEA6}"/>
-    <hyperlink ref="B38" r:id="rId12" xr:uid="{6B4EE0EB-81AB-42A0-96F1-316EBCEB21D3}"/>
-    <hyperlink ref="B40" r:id="rId13" xr:uid="{57589909-C82E-4CCC-AFEC-19027B463B9F}"/>
-    <hyperlink ref="B42" r:id="rId14" xr:uid="{C5CAF0FA-76BF-4F18-8A28-588AF84A19CA}"/>
-    <hyperlink ref="B44" r:id="rId15" xr:uid="{869E4BF5-64BF-4D56-AFDC-1F80324EA37E}"/>
-    <hyperlink ref="B46" r:id="rId16" xr:uid="{F3BD165A-0145-4059-B657-15F962782CAF}"/>
-    <hyperlink ref="B48" r:id="rId17" xr:uid="{AEF02623-BA49-4C21-A4BD-011FA05D2885}"/>
-    <hyperlink ref="B50" r:id="rId18" xr:uid="{4EBB94A4-FDD7-4A12-AC43-9F5CFB7F645A}"/>
-    <hyperlink ref="B14" r:id="rId19" xr:uid="{8603B1A4-55C2-4699-80D4-13543687D8FF}"/>
-    <hyperlink ref="B25" r:id="rId20" xr:uid="{A0C11AAC-F603-4A70-BC64-BE4E56766FE4}"/>
-    <hyperlink ref="B27" r:id="rId21" xr:uid="{B13365A4-8DF0-4D3E-B191-291E1F59A960}"/>
-    <hyperlink ref="B29" r:id="rId22" xr:uid="{C313ED09-CD7D-490E-8452-645CEAF92509}"/>
-    <hyperlink ref="B31" r:id="rId23" xr:uid="{248F266D-528D-4330-BFE7-A2D331417665}"/>
-    <hyperlink ref="B33" r:id="rId24" xr:uid="{8B0ECC09-40F9-4285-A902-7162986C28BB}"/>
-    <hyperlink ref="B35" r:id="rId25" xr:uid="{743E42E0-8041-4BE9-AF8E-B30CA6CB3905}"/>
-    <hyperlink ref="B37" r:id="rId26" xr:uid="{DF1D73B4-783D-43AA-824D-20120DB4EF0F}"/>
-    <hyperlink ref="B39" r:id="rId27" xr:uid="{CAD6712F-B904-4823-A0C0-6B962C57EBC1}"/>
-    <hyperlink ref="B41" r:id="rId28" xr:uid="{4116B2C3-E2BC-442B-A63D-174A8F9D026C}"/>
-    <hyperlink ref="B43" r:id="rId29" xr:uid="{BE37CBAD-3761-4848-9719-B7E46E42F586}"/>
-    <hyperlink ref="B45" r:id="rId30" xr:uid="{AD641D00-9BB7-4C10-A2B6-CFE7420D46D1}"/>
-    <hyperlink ref="B47" r:id="rId31" xr:uid="{1D1B7B64-488A-4335-B512-5EEEED552F41}"/>
-    <hyperlink ref="B49" r:id="rId32" xr:uid="{39BFD6BF-4BB5-4D49-B6F7-3930EE773EB9}"/>
-    <hyperlink ref="B51" r:id="rId33" xr:uid="{5A402808-519E-482D-AD14-7A83D42C69BC}"/>
-    <hyperlink ref="B4:B12" r:id="rId34" display="http://hl7.eu/fhir/hdr/StructureDefinition/condition-eu-hdr" xr:uid="{C99594A2-DC35-4AAA-A8FF-ECEDEC04D888}"/>
-    <hyperlink ref="A3:A51" r:id="rId35" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{4172EE50-327F-4759-9194-4A6A4EE9FE2E}"/>
-    <hyperlink ref="B15:B24" r:id="rId36" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{11465EA0-C892-4233-9CE1-6B6A8996F738}"/>
-    <hyperlink ref="A17" r:id="rId37" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{8035035C-AE47-436D-8B48-21C558EED0A5}"/>
-    <hyperlink ref="B17" r:id="rId38" xr:uid="{2A4586F9-1F5D-414E-B8F1-B8D19F9A848A}"/>
-    <hyperlink ref="A20" r:id="rId39" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{30F0439E-FBEC-4D7E-B5E2-700E8A964891}"/>
-    <hyperlink ref="A21" r:id="rId40" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{BF200BB8-1E27-4530-8E82-94150A84ED43}"/>
-    <hyperlink ref="A22" r:id="rId41" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{D5654463-DF4C-4515-B9DB-D2306C7CF960}"/>
-    <hyperlink ref="A23" r:id="rId42" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{20C4FA90-09C9-4937-98B9-66E0F27465EB}"/>
-    <hyperlink ref="B20" r:id="rId43" xr:uid="{3D502B2E-CCBB-4A8A-B54C-01A771D35ABD}"/>
-    <hyperlink ref="B21" r:id="rId44" xr:uid="{83D53DFB-934E-4F3E-A0CF-EEFACA1940D0}"/>
-    <hyperlink ref="B22" r:id="rId45" xr:uid="{04FDCB16-C035-4EEB-AE40-040219EB6626}"/>
-    <hyperlink ref="B23" r:id="rId46" xr:uid="{CBF6EF75-9B40-4D63-B0F2-5D295D3F47D0}"/>
+    <hyperlink ref="B61" r:id="rId7" xr:uid="{C5CAF0FA-76BF-4F18-8A28-588AF84A19CA}"/>
+    <hyperlink ref="B63" r:id="rId8" xr:uid="{869E4BF5-64BF-4D56-AFDC-1F80324EA37E}"/>
+    <hyperlink ref="B65" r:id="rId9" xr:uid="{F3BD165A-0145-4059-B657-15F962782CAF}"/>
+    <hyperlink ref="B67" r:id="rId10" xr:uid="{AEF02623-BA49-4C21-A4BD-011FA05D2885}"/>
+    <hyperlink ref="B69" r:id="rId11" xr:uid="{4EBB94A4-FDD7-4A12-AC43-9F5CFB7F645A}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{8603B1A4-55C2-4699-80D4-13543687D8FF}"/>
+    <hyperlink ref="B25" r:id="rId13" xr:uid="{A0C11AAC-F603-4A70-BC64-BE4E56766FE4}"/>
+    <hyperlink ref="B35" r:id="rId14" xr:uid="{248F266D-528D-4330-BFE7-A2D331417665}"/>
+    <hyperlink ref="B62" r:id="rId15" xr:uid="{BE37CBAD-3761-4848-9719-B7E46E42F586}"/>
+    <hyperlink ref="B64" r:id="rId16" xr:uid="{AD641D00-9BB7-4C10-A2B6-CFE7420D46D1}"/>
+    <hyperlink ref="B66" r:id="rId17" xr:uid="{1D1B7B64-488A-4335-B512-5EEEED552F41}"/>
+    <hyperlink ref="B68" r:id="rId18" xr:uid="{39BFD6BF-4BB5-4D49-B6F7-3930EE773EB9}"/>
+    <hyperlink ref="B70" r:id="rId19" xr:uid="{5A402808-519E-482D-AD14-7A83D42C69BC}"/>
+    <hyperlink ref="B4:B12" r:id="rId20" display="http://hl7.eu/fhir/hdr/StructureDefinition/condition-eu-hdr" xr:uid="{C99594A2-DC35-4AAA-A8FF-ECEDEC04D888}"/>
+    <hyperlink ref="B15:B24" r:id="rId21" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{11465EA0-C892-4233-9CE1-6B6A8996F738}"/>
+    <hyperlink ref="B17" r:id="rId22" xr:uid="{2A4586F9-1F5D-414E-B8F1-B8D19F9A848A}"/>
+    <hyperlink ref="B20" r:id="rId23" xr:uid="{3D502B2E-CCBB-4A8A-B54C-01A771D35ABD}"/>
+    <hyperlink ref="B21" r:id="rId24" xr:uid="{83D53DFB-934E-4F3E-A0CF-EEFACA1940D0}"/>
+    <hyperlink ref="B22" r:id="rId25" xr:uid="{04FDCB16-C035-4EEB-AE40-040219EB6626}"/>
+    <hyperlink ref="B23" r:id="rId26" xr:uid="{CBF6EF75-9B40-4D63-B0F2-5D295D3F47D0}"/>
+    <hyperlink ref="B27" r:id="rId27" xr:uid="{9B091FB0-6CC8-4F9A-8193-729AE4EDF2DC}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{C48C08DA-3D64-4710-B3F9-5AD75E0FD471}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{CF02B558-F628-451A-8D9B-7E1F1596B565}"/>
+    <hyperlink ref="B30" r:id="rId30" xr:uid="{C1CF2DEF-18A5-436B-B9F8-AE6721E50991}"/>
+    <hyperlink ref="B32" r:id="rId31" xr:uid="{0730299F-D358-46E7-B884-F04B6550243D}"/>
+    <hyperlink ref="B33:B34" r:id="rId32" display="http://hl7.eu/fhir/hdr/StructureDefinition/deviceUseStatement-eu-hdr" xr:uid="{9FC70F59-3C76-420A-9FFB-84F4E3628FE6}"/>
+    <hyperlink ref="B54" r:id="rId33" xr:uid="{41F517A4-054C-41F5-860D-7B046AF4720D}"/>
+    <hyperlink ref="B56" r:id="rId34" xr:uid="{FA628003-6A12-494A-86CD-170EE0657572}"/>
+    <hyperlink ref="B58" r:id="rId35" xr:uid="{79B630C8-F165-45E7-8F67-E87434D3311E}"/>
+    <hyperlink ref="A45" r:id="rId36" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{5DB25E95-03A2-42CE-AFB7-814E6F6A981E}"/>
+    <hyperlink ref="A46:A48" r:id="rId37" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{CD5BC44C-699E-4D18-9279-D84CA1DDBD8A}"/>
+    <hyperlink ref="A49" r:id="rId38" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{A5932BF7-353C-4758-A0EA-3A4253EED4BF}"/>
+    <hyperlink ref="A50:A56" r:id="rId39" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{97E7AD85-6326-45C8-B437-29E440B84A15}"/>
+    <hyperlink ref="A57" r:id="rId40" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{DD64BE54-CFCE-40EF-A9C9-3511FBA5BDB4}"/>
+    <hyperlink ref="A58" r:id="rId41" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{BE1C7E9E-E668-4A0B-8BB0-143FD59B4F81}"/>
+    <hyperlink ref="A59" r:id="rId42" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{9E21F060-2E19-4FBE-8349-E0BEE5E09D00}"/>
+    <hyperlink ref="A60" r:id="rId43" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{4B332FDB-6217-4FCC-8758-04499AFAFDC5}"/>
+    <hyperlink ref="B48" r:id="rId44" xr:uid="{FA2DFF67-DE5E-4244-B6F9-5F8E9941EFE5}"/>
+    <hyperlink ref="B49:B53" r:id="rId45" display="http://hl7.eu/fhir/hdr/StructureDefinition/medication-eu-hdr" xr:uid="{4776D030-54C0-4228-9CCF-CC22BABD8191}"/>
+    <hyperlink ref="B46" r:id="rId46" xr:uid="{D01E7E96-E5B5-4F08-AC0C-E8385DD0BAD6}"/>
+    <hyperlink ref="B55" r:id="rId47" xr:uid="{73E4B839-461A-4DE0-9871-264ED3C87B3E}"/>
+    <hyperlink ref="B57" r:id="rId48" xr:uid="{793159DC-75A3-463A-B510-C434934477EE}"/>
+    <hyperlink ref="B59" r:id="rId49" xr:uid="{62C7241D-6BD1-4EE4-A7DC-722825E30036}"/>
+    <hyperlink ref="B60" r:id="rId50" xr:uid="{6D51D302-A12D-44B7-8219-5B83EC0C90A6}"/>
+    <hyperlink ref="B47" r:id="rId51" xr:uid="{F28C4594-25F3-40A1-A183-75C0B8B6326E}"/>
+    <hyperlink ref="B36" r:id="rId52" xr:uid="{412E3AEF-E2CB-4D5E-AB9F-90DB43AFE5CE}"/>
+    <hyperlink ref="B43" r:id="rId53" xr:uid="{814C1E09-0EF4-4A9B-BE34-6B5D28E43BE5}"/>
+    <hyperlink ref="B37" r:id="rId54" xr:uid="{B69865DF-3192-4A76-89F4-C4183F6A5C02}"/>
+    <hyperlink ref="B42" r:id="rId55" xr:uid="{9C7C38FD-A6D2-4EC6-A8BA-E4C07ABDF006}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16104,8 +16779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -17110,7 +17785,7 @@
         <v>A.2.2 - Alerts</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1224</v>
+        <v>1218</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
@@ -17164,7 +17839,7 @@
         <v>A.2.4 - Admission evaluation</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>1223</v>
+        <v>1217</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
@@ -17191,7 +17866,7 @@
         <v>A.2.5 - Patient history</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>1222</v>
+        <v>1216</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7" t="s">
@@ -17245,7 +17920,7 @@
         <v>A.2.7 - Discharge details</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
@@ -17272,7 +17947,7 @@
         <v>A.2.7.1 - Objective findings</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
@@ -17297,7 +17972,7 @@
         <v>A.2.7.1 - Objective findings</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7" t="s">
@@ -17322,7 +17997,7 @@
         <v>A.2.7.2 - Functional status</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
@@ -17347,7 +18022,7 @@
         <v>A.2.7.2 - Functional status</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
@@ -17372,7 +18047,7 @@
         <v>A.2.7.3 - Discharge note</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
@@ -17397,14 +18072,14 @@
         <v>A.2.8 - Care plan and other recommendations after discharge.</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>1237</v>
+        <v>1231</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -17708,7 +18383,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>1234</v>
+        <v>1228</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
@@ -17718,7 +18393,7 @@
         <v>ObjectiveFindingsHdrEhn</v>
       </c>
       <c r="D12" t="s">
-        <v>1231</v>
+        <v>1225</v>
       </c>
       <c r="E12" t="s">
         <v>107</v>
@@ -17726,7 +18401,7 @@
     </row>
     <row r="13" spans="1:5" ht="59" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>1235</v>
+        <v>1229</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
@@ -17736,15 +18411,15 @@
         <v>FunctionalStatusHdrEhn</v>
       </c>
       <c r="D13" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>1236</v>
+        <v>1230</v>
       </c>
       <c r="B14" t="s">
         <v>83</v>
@@ -17753,7 +18428,7 @@
         <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
       <c r="E14" t="s">
         <v>208</v>
@@ -17778,7 +18453,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>1218</v>
+        <v>1212</v>
       </c>
       <c r="B16" t="s">
         <v>84</v>
@@ -17787,7 +18462,7 @@
         <v>1149</v>
       </c>
       <c r="D16" t="s">
-        <v>1228</v>
+        <v>1222</v>
       </c>
       <c r="E16" t="s">
         <v>691</v>
@@ -17795,7 +18470,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>1219</v>
+        <v>1213</v>
       </c>
       <c r="B17" t="s">
         <v>84</v>
@@ -17804,7 +18479,7 @@
         <v>1150</v>
       </c>
       <c r="D17" t="s">
-        <v>1229</v>
+        <v>1223</v>
       </c>
       <c r="E17" t="s">
         <v>701</v>
@@ -17812,7 +18487,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>1220</v>
+        <v>1214</v>
       </c>
       <c r="B18" t="s">
         <v>84</v>
@@ -17821,7 +18496,7 @@
         <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>1230</v>
+        <v>1224</v>
       </c>
       <c r="E18" t="s">
         <v>708</v>
@@ -18101,7 +18776,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="B2" t="s">
         <v>85</v>
@@ -18118,7 +18793,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
@@ -18135,7 +18810,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -18152,7 +18827,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="B5" t="s">
         <v>85</v>
@@ -18169,7 +18844,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
@@ -18186,7 +18861,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="B7" t="s">
         <v>84</v>
@@ -18203,7 +18878,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -18220,7 +18895,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="B9" t="s">
         <v>85</v>
@@ -18237,7 +18912,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="B10" t="s">
         <v>85</v>
@@ -18254,7 +18929,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
@@ -18271,7 +18946,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="B12" t="s">
         <v>85</v>
@@ -18299,7 +18974,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18357,14 +19032,14 @@
         <v>A.2.8.2.1 - Description</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
@@ -18384,14 +19059,14 @@
         <v>A.2.8.2.1 - Description</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
@@ -18400,7 +19075,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="C4" s="9" t="str">
         <f>LogicalModels!$A$13&amp;"."&amp;FunctionalStatusHdrEhn!A3</f>
@@ -18411,7 +19086,7 @@
         <v>A.2.8.2.2 - Onset Date</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
@@ -18443,7 +19118,7 @@
         <v>20</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
@@ -18468,7 +19143,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
@@ -18493,7 +19168,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
added sdoh, revised maps
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EEA17E-4238-4DA3-8BC3-1914386C5C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04A85FA-9968-4805-BB9F-1023B88FE074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="3" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="1388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="1393">
   <si>
     <t>Group Source</t>
   </si>
@@ -4268,6 +4268,21 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/observation-sdoh-eu-hdr</t>
+  </si>
+  <si>
+    <t>category and code to be defined</t>
+  </si>
+  <si>
+    <t>category to be defined</t>
+  </si>
+  <si>
+    <t>Observation.note</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Observation</t>
   </si>
 </sst>
 </file>
@@ -4426,7 +4441,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4483,11 +4498,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -13930,10 +13941,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -14169,14 +14180,14 @@
         <f xml:space="preserve"> PatientHistoryEhn!D9</f>
         <v>A.2.6.1.1.6 - Resolution circumstances</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="7" t="s">
         <v>1262</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="9" t="s">
         <v>1378</v>
       </c>
     </row>
@@ -14193,14 +14204,14 @@
         <f xml:space="preserve"> PatientHistoryEhn!D9</f>
         <v>A.2.6.1.1.6 - Resolution circumstances</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="7" t="s">
         <v>1377</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="9" t="s">
         <v>1378</v>
       </c>
     </row>
@@ -14224,7 +14235,7 @@
         <v>1269</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -15293,7 +15304,7 @@
         <f xml:space="preserve"> PatientHistoryEhn!D46</f>
         <v>A.2.6.2.1 - Patient relationship</v>
       </c>
-      <c r="E53" s="32" t="s">
+      <c r="E53" s="18" t="s">
         <v>1382</v>
       </c>
       <c r="F53" s="7"/>
@@ -15318,7 +15329,7 @@
         <f xml:space="preserve"> PatientHistoryEhn!D47</f>
         <v>A.2.6.2.2 - Date of birth</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="18" t="s">
         <v>1383</v>
       </c>
       <c r="F54" s="7"/>
@@ -15343,7 +15354,7 @@
         <f xml:space="preserve"> PatientHistoryEhn!D48</f>
         <v>A.2.6.2.3 - Age or date of death</v>
       </c>
-      <c r="E55" s="32" t="s">
+      <c r="E55" s="18" t="s">
         <v>1384</v>
       </c>
       <c r="F55" s="10"/>
@@ -15368,7 +15379,7 @@
         <f xml:space="preserve"> PatientHistoryEhn!D49</f>
         <v>A.2.6.2.5 - Condition</v>
       </c>
-      <c r="E56" s="32" t="s">
+      <c r="E56" s="18" t="s">
         <v>1385</v>
       </c>
       <c r="F56" s="7"/>
@@ -15393,7 +15404,7 @@
         <f xml:space="preserve"> PatientHistoryEhn!D50</f>
         <v>A.2.6.2.6 - Cause of death</v>
       </c>
-      <c r="E57" s="32" t="s">
+      <c r="E57" s="18" t="s">
         <v>1385</v>
       </c>
       <c r="F57" s="7"/>
@@ -15409,7 +15420,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="29" t="s">
         <v>901</v>
       </c>
       <c r="C58" s="9" t="str">
@@ -15434,8 +15445,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B59" s="25" t="s">
-        <v>901</v>
+      <c r="B59" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C59" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A52</f>
@@ -15446,14 +15457,14 @@
         <v>A.2.6.3.1 - Participation in society</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>1223</v>
+        <v>1338</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>1358</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.75">
@@ -15461,8 +15472,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B60" s="25" t="s">
-        <v>901</v>
+      <c r="B60" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C60" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A53</f>
@@ -15473,14 +15484,14 @@
         <v>A.2.6.3.1.1 - Work situation</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.75">
@@ -15488,8 +15499,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B61" s="25" t="s">
-        <v>901</v>
+      <c r="B61" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C61" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A54</f>
@@ -15500,14 +15511,14 @@
         <v>A.2.6.3.1.2 - Hobby</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.75">
@@ -15515,8 +15526,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B62" s="25" t="s">
-        <v>901</v>
+      <c r="B62" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C62" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A55</f>
@@ -15527,14 +15538,14 @@
         <v>A.2.6.3.1.3 - Social network</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.75">
@@ -15542,8 +15553,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B63" s="25" t="s">
-        <v>901</v>
+      <c r="B63" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C63" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A56</f>
@@ -15554,14 +15565,14 @@
         <v>A.2.6.3.2 - Education</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>1223</v>
+        <v>1338</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>1358</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.75">
@@ -15569,8 +15580,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B64" s="25" t="s">
-        <v>901</v>
+      <c r="B64" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C64" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A57</f>
@@ -15581,14 +15592,14 @@
         <v>A.2.6.3.2.1 - Education level</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.75">
@@ -15596,8 +15607,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B65" s="25" t="s">
-        <v>901</v>
+      <c r="B65" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C65" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A58</f>
@@ -15608,14 +15619,14 @@
         <v>A.2.6.3.2.2 - Comment</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>1223</v>
+        <v>1391</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H65" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.75">
@@ -15623,8 +15634,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B66" s="25" t="s">
-        <v>901</v>
+      <c r="B66" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C66" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A59</f>
@@ -15635,14 +15646,14 @@
         <v>A.2.6.3.3 - Living situation</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>1223</v>
+        <v>1338</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H66" s="14" t="s">
-        <v>1358</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.75">
@@ -15650,8 +15661,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B67" s="25" t="s">
-        <v>901</v>
+      <c r="B67" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C67" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A60</f>
@@ -15662,14 +15673,14 @@
         <v>A.2.6.3.3.1 - House type</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.75">
@@ -15677,8 +15688,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B68" s="25" t="s">
-        <v>901</v>
+      <c r="B68" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C68" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A61</f>
@@ -15689,14 +15700,14 @@
         <v>A.2.6.3.3.2 - Home adaption</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.75">
@@ -15704,8 +15715,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B69" s="25" t="s">
-        <v>901</v>
+      <c r="B69" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C69" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A62</f>
@@ -15716,14 +15727,14 @@
         <v>A.2.6.3.3.3 - Living conditions</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.75">
@@ -15731,8 +15742,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B70" s="25" t="s">
-        <v>901</v>
+      <c r="B70" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C70" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A63</f>
@@ -15743,14 +15754,14 @@
         <v>A.2.6.3.4 - Family situation</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>1223</v>
+        <v>1338</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>1358</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.75">
@@ -15758,8 +15769,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B71" s="25" t="s">
-        <v>901</v>
+      <c r="B71" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C71" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A64</f>
@@ -15770,14 +15781,14 @@
         <v>A.2.6.3.4.1 - Comment</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.75">
@@ -15785,8 +15796,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B72" s="25" t="s">
-        <v>901</v>
+      <c r="B72" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C72" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A65</f>
@@ -15797,14 +15808,14 @@
         <v>A.2.6.3.4.2 - Family composition</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.75">
@@ -15812,8 +15823,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B73" s="25" t="s">
-        <v>901</v>
+      <c r="B73" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C73" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A66</f>
@@ -15824,14 +15835,14 @@
         <v>A.2.6.3.4.3 - Marital status</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.75">
@@ -15839,8 +15850,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B74" s="25" t="s">
-        <v>901</v>
+      <c r="B74" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C74" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A67</f>
@@ -15851,23 +15862,23 @@
         <v>A.2.6.3.4.4 - Number of children</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A75" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B75" s="25" t="s">
-        <v>901</v>
+      <c r="B75" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C75" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A68</f>
@@ -15878,14 +15889,14 @@
         <v>A.2.6.3.4.5 - Number of children at home</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.75">
@@ -15893,8 +15904,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B76" s="25" t="s">
-        <v>901</v>
+      <c r="B76" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C76" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A69</f>
@@ -15905,14 +15916,14 @@
         <v>A.2.6.3.4.6 - Child details</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.75">
@@ -15920,8 +15931,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
-      <c r="B77" s="25" t="s">
-        <v>901</v>
+      <c r="B77" s="26" t="s">
+        <v>1388</v>
       </c>
       <c r="C77" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A70</f>
@@ -15932,14 +15943,14 @@
         <v>A.2.6.3.4.7 - Care responsibility</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.75">
@@ -15959,7 +15970,7 @@
         <v>A.2.6.4 - Use of substances</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>1223</v>
+        <v>1367</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="13" t="s">
@@ -15975,7 +15986,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>901</v>
+        <v>1392</v>
       </c>
       <c r="C79" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A72</f>
@@ -15986,14 +15997,14 @@
         <v>A.2.6.4.1 - Alcohol use</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>1223</v>
+        <v>1338</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>1358</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.75">
@@ -16002,7 +16013,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>901</v>
+        <v>1392</v>
       </c>
       <c r="C80" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A73</f>
@@ -16013,91 +16024,355 @@
         <v>A.2.6.4.1.1 - Status</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>1223</v>
+        <v>1342</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D83"/>
-      <c r="H83"/>
-    </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D84"/>
-      <c r="H84"/>
-    </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D85"/>
-      <c r="H85"/>
-    </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D86"/>
-      <c r="H86"/>
-    </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D87"/>
-      <c r="H87"/>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D88"/>
-      <c r="H88"/>
-    </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D89"/>
-      <c r="H89"/>
-    </row>
-    <row r="90" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D90"/>
-      <c r="H90"/>
-    </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="D91"/>
-      <c r="H91"/>
-    </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.75">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A81" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C81" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A74</f>
+        <v>PatientHistory.useOfSubstances.alcohol.periodAndQuantity</v>
+      </c>
+      <c r="D81" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D74</f>
+        <v>A.2.6.4.1.2 - Period and quantity</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F81" s="7"/>
+      <c r="G81" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A82" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C82" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A75</f>
+        <v>PatientHistory.useOfSubstances.alcohol.comment</v>
+      </c>
+      <c r="D82" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D75</f>
+        <v>A.2.6.4.1.3 - Comment</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F82" s="7"/>
+      <c r="G82" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A83" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B83" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C83" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A76</f>
+        <v>PatientHistory.useOfSubstances.tobacco</v>
+      </c>
+      <c r="D83" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D76</f>
+        <v>A.2.6.4.2 - Tobacco use</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F83" s="7"/>
+      <c r="G83" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A84" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B84" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C84" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A77</f>
+        <v>PatientHistory.useOfSubstances.tobacco.currentStatus</v>
+      </c>
+      <c r="D84" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D77</f>
+        <v>A.2.6.4.2.1 - Status</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A85" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C85" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A78</f>
+        <v>PatientHistory.useOfSubstances.tobacco.periodAndQuantity</v>
+      </c>
+      <c r="D85" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D78</f>
+        <v>A.2.6.4.2.2 - Period and quantity</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A86" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B86" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C86" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A79</f>
+        <v>PatientHistory.useOfSubstances.tobacco.comment</v>
+      </c>
+      <c r="D86" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D79</f>
+        <v>A.2.6.4.2.3 - Comment</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A87" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B87" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C87" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A80</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption</v>
+      </c>
+      <c r="D87" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D80</f>
+        <v>A.2.6.4.3 - Drug consumption</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F87" s="7"/>
+      <c r="G87" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H87" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A88" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B88" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C88" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A81</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption.currentStatus</v>
+      </c>
+      <c r="D88" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D81</f>
+        <v>A.2.6.4.3.1 - Status</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A89" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C89" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A82</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption.periodAndQuantity</v>
+      </c>
+      <c r="D89" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D82</f>
+        <v>A.2.6.4.3.2 - Period and quantity</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A90" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B90" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C90" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A83</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption.drugType</v>
+      </c>
+      <c r="D90" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D83</f>
+        <v>A.2.6.4.3.3 - Drug or medication type</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F90" s="7"/>
+      <c r="G90" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H90" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A91" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B91" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C91" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A84</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption.route</v>
+      </c>
+      <c r="D91" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D84</f>
+        <v>A.2.6.4.3.4 - Route of administration</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H91" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A92" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+      </c>
+      <c r="B92" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C92" s="9" t="str">
+        <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A85</f>
+        <v>PatientHistory.useOfSubstances.drugConsumption.comment</v>
+      </c>
+      <c r="D92" s="9" t="str">
+        <f xml:space="preserve"> PatientHistoryEhn!D85</f>
+        <v>A.2.6.4.3.5 - Comment</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.75">
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.75">
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C95" s="30"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
-    </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.75">
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-    </row>
-    <row r="97" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-    </row>
-    <row r="98" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-    </row>
-    <row r="99" spans="5:7" x14ac:dyDescent="0.75">
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -16138,9 +16413,25 @@
     <hyperlink ref="B53" r:id="rId35" xr:uid="{0EFC7461-5DD0-4A27-AAB7-B1D239101879}"/>
     <hyperlink ref="B10" r:id="rId36" xr:uid="{B7274725-2394-49DA-802C-BEB611C56196}"/>
     <hyperlink ref="B54:B57" r:id="rId37" display="http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr" xr:uid="{9886B42D-1BC0-4839-8F10-E5E29C29F906}"/>
+    <hyperlink ref="B59" r:id="rId38" xr:uid="{1BD66CD8-805B-4C66-A27F-A17FB6FC6822}"/>
+    <hyperlink ref="B60:B77" r:id="rId39" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-sdoh-eu-hdr" xr:uid="{52780DF2-8707-430C-BC90-180EB00C41FE}"/>
+    <hyperlink ref="A81" r:id="rId40" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{A2E34487-E225-44F3-8445-926F141986AC}"/>
+    <hyperlink ref="A82" r:id="rId41" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{176AC99F-6325-4718-91DF-404F2AC0208B}"/>
+    <hyperlink ref="A83" r:id="rId42" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{99AC7EEE-2B09-4FB9-AC39-FA4FB1C1BFE7}"/>
+    <hyperlink ref="A84" r:id="rId43" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C051815A-D8B0-4A1E-B650-BF6B87B7F726}"/>
+    <hyperlink ref="A85" r:id="rId44" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{ED7E8E50-5B82-4B05-A075-9A8F5FAC56D0}"/>
+    <hyperlink ref="A86" r:id="rId45" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{0F134206-F76A-49E3-8C8C-67012A6C7EDA}"/>
+    <hyperlink ref="A87" r:id="rId46" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C7CB330D-8622-481D-8BBE-FCDE98F65BD6}"/>
+    <hyperlink ref="A88" r:id="rId47" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{84C08D75-9402-41E0-9794-E25CA68F7EED}"/>
+    <hyperlink ref="A89" r:id="rId48" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{877EEB89-DAA9-4CEF-9E21-3B7D51D217AB}"/>
+    <hyperlink ref="A90" r:id="rId49" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{09487E9D-B0D4-49B8-BB7F-326DFF9F09D5}"/>
+    <hyperlink ref="A91" r:id="rId50" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{956192D1-715C-43EA-8651-5618321D7AC2}"/>
+    <hyperlink ref="A92" r:id="rId51" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{855B8AED-9EBD-4A80-A895-DCA49F7463D5}"/>
+    <hyperlink ref="B79" r:id="rId52" xr:uid="{97E4BABB-9515-4E6B-BEAB-B137F7A3DA10}"/>
+    <hyperlink ref="B80:B92" r:id="rId53" display="http://hl7.org/fhir/StructureDefinition/Observation" xr:uid="{66FB3999-651C-4EE5-8E40-E7B880188A34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -16148,9 +16439,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="63.04296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.76953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
@@ -17869,14 +18165,14 @@
         <f xml:space="preserve"> HospitalStayEhn!D10</f>
         <v>A.2.7.1.8 - Resolution circumstances</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="7" t="s">
         <v>1262</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="9" t="s">
         <v>1378</v>
       </c>
     </row>
@@ -17893,14 +18189,14 @@
         <f xml:space="preserve"> HospitalStayEhn!D10</f>
         <v>A.2.7.1.8 - Resolution circumstances</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="9" t="s">
         <v>1377</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="9" t="s">
         <v>1378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added infection exposure from xpandh
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04A85FA-9968-4805-BB9F-1023B88FE074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959B8D11-865C-4E6D-9E0B-96760DB1D63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="3" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="1395">
   <si>
     <t>Group Source</t>
   </si>
@@ -4283,6 +4283,12 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/StructureDefinition/Observation</t>
+  </si>
+  <si>
+    <t>If it refer to the usage period</t>
+  </si>
+  <si>
+    <t>if the implantation procedure date is recorded</t>
   </si>
 </sst>
 </file>
@@ -13943,8 +13949,8 @@
   </sheetPr>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -17905,8 +17911,8 @@
   </sheetPr>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="B17" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18298,7 +18304,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="9"/>
     </row>
@@ -18400,7 +18406,7 @@
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="9"/>
     </row>
@@ -18500,7 +18506,7 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="9"/>
     </row>
@@ -18523,8 +18529,8 @@
       <c r="E24" s="9" t="s">
         <v>1291</v>
       </c>
-      <c r="G24" s="22" t="s">
-        <v>22</v>
+      <c r="G24" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="H24" s="23"/>
     </row>
@@ -18712,7 +18718,7 @@
         <v>22</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>1307</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
@@ -18739,7 +18745,7 @@
         <v>22</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>1311</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
fixed all the QA model mapping errors
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF8D3D1-9F08-4351-BD86-278D0C557FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1099D1-2847-435D-98A7-4ED9802AA844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="IG-groups" sheetId="31" r:id="rId1"/>
@@ -7717,7 +7717,7 @@
   <dimension ref="A1:AZ16"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8350,8 +8350,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -14450,8 +14450,8 @@
   </sheetPr>
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -14494,8 +14494,8 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>862</v>
@@ -14521,8 +14521,8 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>862</v>
@@ -14548,8 +14548,8 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>1191</v>
@@ -14573,8 +14573,8 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>1191</v>
@@ -14598,8 +14598,8 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>1191</v>
@@ -14623,8 +14623,8 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>1191</v>
@@ -14648,8 +14648,8 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>1191</v>
@@ -14673,8 +14673,8 @@
     </row>
     <row r="9" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A9" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>1191</v>
@@ -14699,7 +14699,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A10" s="8"/>
+      <c r="A10" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B10" s="8" t="s">
         <v>862</v>
       </c>
@@ -14724,8 +14727,8 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>1191</v>
@@ -14748,8 +14751,8 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1191</v>
@@ -14773,8 +14776,8 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>862</v>
@@ -14798,8 +14801,8 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>1234</v>
@@ -14824,7 +14827,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A15" s="8"/>
+      <c r="A15" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B15" s="8" t="s">
         <v>1220</v>
       </c>
@@ -14849,8 +14855,8 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>1220</v>
@@ -14875,7 +14881,10 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A17" s="8"/>
+      <c r="A17" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B17" s="8" t="s">
         <v>1220</v>
       </c>
@@ -14900,8 +14909,8 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>1234</v>
@@ -14926,7 +14935,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A19" s="8"/>
+      <c r="A19" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B19" s="8" t="s">
         <v>1206</v>
       </c>
@@ -14951,8 +14963,8 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>1234</v>
@@ -14976,8 +14988,8 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>1234</v>
@@ -15003,8 +15015,8 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>1234</v>
@@ -15028,8 +15040,8 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>1234</v>
@@ -15053,8 +15065,8 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>1206</v>
@@ -15078,8 +15090,8 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>1206</v>
@@ -15103,8 +15115,8 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>1206</v>
@@ -15127,7 +15139,10 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A27" s="8"/>
+      <c r="A27" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B27" s="11" t="s">
         <v>1206</v>
       </c>
@@ -15152,8 +15167,8 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>1206</v>
@@ -15177,8 +15192,8 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>1206</v>
@@ -15201,7 +15216,10 @@
       <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A30" s="8"/>
+      <c r="A30" s="8" t="str">
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
+      </c>
       <c r="B30" s="11" t="s">
         <v>1206</v>
       </c>
@@ -15224,8 +15242,8 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>1206</v>
@@ -15249,8 +15267,8 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>1206</v>
@@ -15274,8 +15292,8 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A33" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>862</v>
@@ -15299,8 +15317,8 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>1292</v>
@@ -15323,8 +15341,8 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A35" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>1292</v>
@@ -15348,8 +15366,8 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A36" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>1292</v>
@@ -15373,8 +15391,8 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A37" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>1292</v>
@@ -15398,8 +15416,8 @@
     </row>
     <row r="38" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A38" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>1292</v>
@@ -15423,8 +15441,8 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A39" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>1292</v>
@@ -15448,8 +15466,8 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A40" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>1293</v>
@@ -15473,8 +15491,8 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A41" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B41" s="23" t="s">
         <v>862</v>
@@ -15500,8 +15518,8 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A42" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>862</v>
@@ -15525,8 +15543,8 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A43" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>1317</v>
@@ -15550,8 +15568,8 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A44" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>1317</v>
@@ -15577,8 +15595,8 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A45" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>1317</v>
@@ -15604,8 +15622,8 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A46" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B46" s="24" t="s">
         <v>1317</v>
@@ -15631,8 +15649,8 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A47" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>1317</v>
@@ -15656,8 +15674,8 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A48" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>862</v>
@@ -15681,8 +15699,8 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A49" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>1321</v>
@@ -15706,8 +15724,8 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A50" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B50" s="24" t="s">
         <v>1321</v>
@@ -15731,8 +15749,8 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A51" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>1321</v>
@@ -15756,8 +15774,8 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A52" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>862</v>
@@ -15781,8 +15799,8 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A53" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B53" s="24" t="s">
         <v>1380</v>
@@ -15806,8 +15824,8 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A54" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>1380</v>
@@ -15831,8 +15849,8 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A55" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B55" s="24" t="s">
         <v>1380</v>
@@ -15856,8 +15874,8 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A56" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B56" s="24" t="s">
         <v>1380</v>
@@ -15881,8 +15899,8 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A57" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>1380</v>
@@ -15908,8 +15926,8 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A58" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>862</v>
@@ -15933,8 +15951,8 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A59" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>1309</v>
@@ -15960,8 +15978,8 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A60" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>1309</v>
@@ -15987,8 +16005,8 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A61" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B61" s="24" t="s">
         <v>1309</v>
@@ -16014,8 +16032,8 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A62" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>1309</v>
@@ -16041,8 +16059,8 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A63" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B63" s="24" t="s">
         <v>1309</v>
@@ -16068,8 +16086,8 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A64" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B64" s="24" t="s">
         <v>1309</v>
@@ -16095,8 +16113,8 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A65" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B65" s="24" t="s">
         <v>1309</v>
@@ -16122,8 +16140,8 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A66" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>1309</v>
@@ -16149,8 +16167,8 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A67" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B67" s="24" t="s">
         <v>1309</v>
@@ -16176,8 +16194,8 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A68" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B68" s="24" t="s">
         <v>1309</v>
@@ -16203,8 +16221,8 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A69" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B69" s="24" t="s">
         <v>1309</v>
@@ -16230,8 +16248,8 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A70" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B70" s="24" t="s">
         <v>1309</v>
@@ -16257,8 +16275,8 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A71" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B71" s="24" t="s">
         <v>1309</v>
@@ -16284,8 +16302,8 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A72" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B72" s="24" t="s">
         <v>1309</v>
@@ -16311,8 +16329,8 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A73" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B73" s="24" t="s">
         <v>1309</v>
@@ -16338,8 +16356,8 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A74" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B74" s="24" t="s">
         <v>1309</v>
@@ -16365,8 +16383,8 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A75" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B75" s="24" t="s">
         <v>1309</v>
@@ -16392,8 +16410,8 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A76" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B76" s="24" t="s">
         <v>1309</v>
@@ -16419,8 +16437,8 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A77" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B77" s="24" t="s">
         <v>1309</v>
@@ -16446,8 +16464,8 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A78" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B78" s="23" t="s">
         <v>862</v>
@@ -16473,8 +16491,8 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A79" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B79" s="23" t="s">
         <v>1313</v>
@@ -16500,8 +16518,8 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A80" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B80" s="23" t="s">
         <v>1313</v>
@@ -16527,8 +16545,8 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A81" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B81" s="23" t="s">
         <v>1313</v>
@@ -16554,8 +16572,8 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A82" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B82" s="23" t="s">
         <v>1313</v>
@@ -16581,8 +16599,8 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A83" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B83" s="23" t="s">
         <v>1313</v>
@@ -16608,8 +16626,8 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A84" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B84" s="23" t="s">
         <v>1313</v>
@@ -16635,8 +16653,8 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A85" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B85" s="23" t="s">
         <v>1313</v>
@@ -16662,8 +16680,8 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A86" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B86" s="23" t="s">
         <v>1313</v>
@@ -16689,8 +16707,8 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A87" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B87" s="23" t="s">
         <v>1313</v>
@@ -16716,8 +16734,8 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A88" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B88" s="23" t="s">
         <v>1313</v>
@@ -16743,8 +16761,8 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A89" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B89" s="23" t="s">
         <v>1313</v>
@@ -16770,8 +16788,8 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A90" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B90" s="23" t="s">
         <v>1313</v>
@@ -16797,8 +16815,8 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A91" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B91" s="23" t="s">
         <v>1313</v>
@@ -16824,8 +16842,8 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A92" s="8" t="str">
-        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$B$9</f>
-        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistoryEhn</v>
+        <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
+        <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
       <c r="B92" s="23" t="s">
         <v>1313</v>
@@ -16867,60 +16885,41 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A5" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{D83C9D87-A7B7-4B4C-BC51-73FADD8E0EAF}"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{773F9F15-3968-4637-9522-7B7E87FE4B08}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{6C3B6166-ED07-4BA3-A6B6-317118974852}"/>
-    <hyperlink ref="B18:B31" r:id="rId4" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{1BFAF02C-82BE-4D51-8BC7-5F7073B14112}"/>
-    <hyperlink ref="B25" r:id="rId5" xr:uid="{5D25BABD-CD16-4F37-9680-8A9077AE0EE0}"/>
-    <hyperlink ref="B26" r:id="rId6" xr:uid="{F3F51840-D7BD-463C-B909-85709D9B7D0C}"/>
-    <hyperlink ref="A3:A71" r:id="rId7" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{FBC4300C-4B6A-47D8-A245-52563758714C}"/>
-    <hyperlink ref="A72:A75" r:id="rId8" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{159D5253-6906-4703-A28F-547A20CA3F2B}"/>
-    <hyperlink ref="A72" r:id="rId9" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C35C6822-0C83-4288-B945-D2845B268AED}"/>
-    <hyperlink ref="A73:A80" r:id="rId10" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C71872E2-E861-4220-A5C7-C292D1A5CC37}"/>
-    <hyperlink ref="B3" r:id="rId11" xr:uid="{D8EE0090-E0A5-4EF2-A4D4-FF298A9EC839}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{2FD40B49-61D5-4FDD-BC10-E24E0C2B7128}"/>
-    <hyperlink ref="B13" r:id="rId13" xr:uid="{898B89C3-468A-4749-9457-FF6A02374DD6}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{39C097E2-7256-4B28-862E-2C842FDEE7BB}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{6DB328AF-296D-4B1F-97EE-3E8938965CDF}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{FFF9FD4D-404C-43C7-B250-B0FBDC924FD2}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{16B99D2A-5DBE-48B3-9925-E99FF8AEDC2C}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{56520413-41EB-4ACB-9DA5-40F1862E94F2}"/>
-    <hyperlink ref="B21:B23" r:id="rId19" display="http://hl7.eu/fhir/hdr/StructureDefinition/deviceUseStatement-eu-hdr" xr:uid="{10B98CC8-FB87-41D5-8E02-1101E71BD8BF}"/>
-    <hyperlink ref="B22" r:id="rId20" xr:uid="{CCC94832-88F5-44D6-B4D5-9DB55D5D4A35}"/>
-    <hyperlink ref="A22" r:id="rId21" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{543268D7-9BE4-4B68-AE4F-AA1F005415E3}"/>
-    <hyperlink ref="B27:B32" r:id="rId22" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{E1EBC81A-61FD-4DC4-B42D-AD1EF86C1E9A}"/>
-    <hyperlink ref="B41" r:id="rId23" xr:uid="{0C2E8B8F-4BC7-4A14-89C9-53D8E0578F3C}"/>
-    <hyperlink ref="A1" r:id="rId24" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{B62B2D10-218E-4A91-B4A9-C4C092E378B9}"/>
-    <hyperlink ref="B34:B40" r:id="rId25" display="http://hl7.eu/fhir/hdr/StructureDefinition/immunization-eu-eps" xr:uid="{A35CA130-777D-4E79-9924-81D156F76728}"/>
-    <hyperlink ref="B33" r:id="rId26" xr:uid="{31535991-099F-4941-BFF8-F5F167C4BFF8}"/>
-    <hyperlink ref="B40" r:id="rId27" display="http://hl7.eu/fhir/hdr/StructureDefinition/ImmunizationRecommendation-eu-eps" xr:uid="{5B125149-4E6A-46A9-BDF2-63A465796C51}"/>
-    <hyperlink ref="B48" r:id="rId28" xr:uid="{27DCBFBF-6884-49AB-B32F-532A98500976}"/>
-    <hyperlink ref="B53" r:id="rId29" display="http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr" xr:uid="{0EFC7461-5DD0-4A27-AAB7-B1D239101879}"/>
-    <hyperlink ref="B10" r:id="rId30" xr:uid="{B7274725-2394-49DA-802C-BEB611C56196}"/>
-    <hyperlink ref="B54:B57" r:id="rId31" display="http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr" xr:uid="{9886B42D-1BC0-4839-8F10-E5E29C29F906}"/>
-    <hyperlink ref="B59" r:id="rId32" xr:uid="{1BD66CD8-805B-4C66-A27F-A17FB6FC6822}"/>
-    <hyperlink ref="B60:B77" r:id="rId33" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-sdoh-eu-hdr" xr:uid="{52780DF2-8707-430C-BC90-180EB00C41FE}"/>
-    <hyperlink ref="A81" r:id="rId34" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{A2E34487-E225-44F3-8445-926F141986AC}"/>
-    <hyperlink ref="A82" r:id="rId35" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{176AC99F-6325-4718-91DF-404F2AC0208B}"/>
-    <hyperlink ref="A83" r:id="rId36" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{99AC7EEE-2B09-4FB9-AC39-FA4FB1C1BFE7}"/>
-    <hyperlink ref="A84" r:id="rId37" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C051815A-D8B0-4A1E-B650-BF6B87B7F726}"/>
-    <hyperlink ref="A85" r:id="rId38" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{ED7E8E50-5B82-4B05-A075-9A8F5FAC56D0}"/>
-    <hyperlink ref="A86" r:id="rId39" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{0F134206-F76A-49E3-8C8C-67012A6C7EDA}"/>
-    <hyperlink ref="A87" r:id="rId40" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{C7CB330D-8622-481D-8BBE-FCDE98F65BD6}"/>
-    <hyperlink ref="A88" r:id="rId41" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{84C08D75-9402-41E0-9794-E25CA68F7EED}"/>
-    <hyperlink ref="A89" r:id="rId42" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{877EEB89-DAA9-4CEF-9E21-3B7D51D217AB}"/>
-    <hyperlink ref="A90" r:id="rId43" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{09487E9D-B0D4-49B8-BB7F-326DFF9F09D5}"/>
-    <hyperlink ref="A91" r:id="rId44" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{956192D1-715C-43EA-8651-5618321D7AC2}"/>
-    <hyperlink ref="A92" r:id="rId45" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{855B8AED-9EBD-4A80-A895-DCA49F7463D5}"/>
-    <hyperlink ref="B79" r:id="rId46" xr:uid="{97E4BABB-9515-4E6B-BEAB-B137F7A3DA10}"/>
-    <hyperlink ref="B80:B92" r:id="rId47" display="http://hl7.org/fhir/StructureDefinition/Observation" xr:uid="{66FB3999-651C-4EE5-8E40-E7B880188A34}"/>
-    <hyperlink ref="B43:B47" r:id="rId48" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-infectious-contact-eu-hdr" xr:uid="{672072C9-55AC-43AB-AD96-6CB816470882}"/>
-    <hyperlink ref="B42" r:id="rId49" xr:uid="{B7B5D1E1-FD79-4072-B1AD-300ADBC1B742}"/>
-    <hyperlink ref="B49" r:id="rId50" xr:uid="{EEA12990-EFB9-47DF-8755-4380013D68D1}"/>
-    <hyperlink ref="B50:B51" r:id="rId51" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-travel-eu-hdr" xr:uid="{62C156D6-503D-47DC-932C-8810EA1276A5}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6C3B6166-ED07-4BA3-A6B6-317118974852}"/>
+    <hyperlink ref="B18:B31" r:id="rId2" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{1BFAF02C-82BE-4D51-8BC7-5F7073B14112}"/>
+    <hyperlink ref="B25" r:id="rId3" xr:uid="{5D25BABD-CD16-4F37-9680-8A9077AE0EE0}"/>
+    <hyperlink ref="B26" r:id="rId4" xr:uid="{F3F51840-D7BD-463C-B909-85709D9B7D0C}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{D8EE0090-E0A5-4EF2-A4D4-FF298A9EC839}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{2FD40B49-61D5-4FDD-BC10-E24E0C2B7128}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{898B89C3-468A-4749-9457-FF6A02374DD6}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{39C097E2-7256-4B28-862E-2C842FDEE7BB}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{6DB328AF-296D-4B1F-97EE-3E8938965CDF}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{FFF9FD4D-404C-43C7-B250-B0FBDC924FD2}"/>
+    <hyperlink ref="B18" r:id="rId11" xr:uid="{16B99D2A-5DBE-48B3-9925-E99FF8AEDC2C}"/>
+    <hyperlink ref="B20" r:id="rId12" xr:uid="{56520413-41EB-4ACB-9DA5-40F1862E94F2}"/>
+    <hyperlink ref="B21:B23" r:id="rId13" display="http://hl7.eu/fhir/hdr/StructureDefinition/deviceUseStatement-eu-hdr" xr:uid="{10B98CC8-FB87-41D5-8E02-1101E71BD8BF}"/>
+    <hyperlink ref="B22" r:id="rId14" xr:uid="{CCC94832-88F5-44D6-B4D5-9DB55D5D4A35}"/>
+    <hyperlink ref="B27:B32" r:id="rId15" display="http://hl7.eu/fhir/hdr/StructureDefinition/procedure-eu-hdr" xr:uid="{E1EBC81A-61FD-4DC4-B42D-AD1EF86C1E9A}"/>
+    <hyperlink ref="B41" r:id="rId16" xr:uid="{0C2E8B8F-4BC7-4A14-89C9-53D8E0578F3C}"/>
+    <hyperlink ref="A1" r:id="rId17" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{B62B2D10-218E-4A91-B4A9-C4C092E378B9}"/>
+    <hyperlink ref="B34:B40" r:id="rId18" display="http://hl7.eu/fhir/hdr/StructureDefinition/immunization-eu-eps" xr:uid="{A35CA130-777D-4E79-9924-81D156F76728}"/>
+    <hyperlink ref="B33" r:id="rId19" xr:uid="{31535991-099F-4941-BFF8-F5F167C4BFF8}"/>
+    <hyperlink ref="B40" r:id="rId20" display="http://hl7.eu/fhir/hdr/StructureDefinition/ImmunizationRecommendation-eu-eps" xr:uid="{5B125149-4E6A-46A9-BDF2-63A465796C51}"/>
+    <hyperlink ref="B48" r:id="rId21" xr:uid="{27DCBFBF-6884-49AB-B32F-532A98500976}"/>
+    <hyperlink ref="B53" r:id="rId22" display="http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr" xr:uid="{0EFC7461-5DD0-4A27-AAB7-B1D239101879}"/>
+    <hyperlink ref="B10" r:id="rId23" xr:uid="{B7274725-2394-49DA-802C-BEB611C56196}"/>
+    <hyperlink ref="B54:B57" r:id="rId24" display="http://hl7.org/fhir/StructureDefinition/familyMemberHistory-eu-hdr" xr:uid="{9886B42D-1BC0-4839-8F10-E5E29C29F906}"/>
+    <hyperlink ref="B59" r:id="rId25" xr:uid="{1BD66CD8-805B-4C66-A27F-A17FB6FC6822}"/>
+    <hyperlink ref="B60:B77" r:id="rId26" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-sdoh-eu-hdr" xr:uid="{52780DF2-8707-430C-BC90-180EB00C41FE}"/>
+    <hyperlink ref="B79" r:id="rId27" xr:uid="{97E4BABB-9515-4E6B-BEAB-B137F7A3DA10}"/>
+    <hyperlink ref="B80:B92" r:id="rId28" display="http://hl7.org/fhir/StructureDefinition/Observation" xr:uid="{66FB3999-651C-4EE5-8E40-E7B880188A34}"/>
+    <hyperlink ref="B43:B47" r:id="rId29" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-infectious-contact-eu-hdr" xr:uid="{672072C9-55AC-43AB-AD96-6CB816470882}"/>
+    <hyperlink ref="B42" r:id="rId30" xr:uid="{B7B5D1E1-FD79-4072-B1AD-300ADBC1B742}"/>
+    <hyperlink ref="B49" r:id="rId31" xr:uid="{EEA12990-EFB9-47DF-8755-4380013D68D1}"/>
+    <hyperlink ref="B50:B51" r:id="rId32" display="http://hl7.eu/fhir/hdr/StructureDefinition/observation-travel-eu-hdr" xr:uid="{62C156D6-503D-47DC-932C-8810EA1276A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
 
@@ -16928,7 +16927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -18396,8 +18395,8 @@
   </sheetPr>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView topLeftCell="C42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:D32"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
fixed duplication of titles and other typos
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEADF65C-4B95-45A5-8F16-834D01FB4657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E34A92-461A-4C64-B0B7-F16FB01402B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="IG-groups" sheetId="31" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3247" uniqueCount="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3247" uniqueCount="1387">
   <si>
     <t>Group Source</t>
   </si>
@@ -4277,6 +4277,9 @@
   </si>
   <si>
     <t>http://hl7.eu/fhir/hdr/StructureDefinition/immunizationRecommendation-eu-hdr</t>
+  </si>
+  <si>
+    <t>eHN Patient History Model to this guide Map</t>
   </si>
 </sst>
 </file>
@@ -7714,10 +7717,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:AZ16"/>
+  <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8218,7 +8221,7 @@
         <v>http://hl7.eu/fhir/hdr/ConceptMap/patientHistory2FHIR-eu-hdr</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1203</v>
+        <v>1386</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>1204</v>
@@ -8312,6 +8315,9 @@
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.75">
       <c r="A16" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.75">
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14196,7 +14202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed obsolete comments in the maps
</commit_message>
<xml_diff>
--- a/models-src/hl7-hdr-models-and-maps.xlsx
+++ b/models-src/hl7-hdr-models-and-maps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-hdr\models-src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zFHIR-publication\hl7-eu\hdr\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E34A92-461A-4C64-B0B7-F16FB01402B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3761E899-09FB-4563-B55F-A34B87961B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="20" activeTab="27" xr2:uid="{FA01C668-562A-4AF9-BDB0-B212F14DE883}"/>
   </bookViews>
   <sheets>
     <sheet name="IG-groups" sheetId="31" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3247" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3237" uniqueCount="1383">
   <si>
     <t>Group Source</t>
   </si>
@@ -4131,9 +4131,6 @@
     <t>Observation.effectiveDateTime</t>
   </si>
   <si>
-    <t>Check if this is part of the Vital Signs or not</t>
-  </si>
-  <si>
     <t>Composition.section:sectionVitalSigns</t>
   </si>
   <si>
@@ -4146,9 +4143,6 @@
     <t>http://hl7.org/fhir/StructureDefinition/vitalsigns</t>
   </si>
   <si>
-    <t>check if a more specialized profile is needed</t>
-  </si>
-  <si>
     <t>ObjectiveFindings2FHIREuHdr</t>
   </si>
   <si>
@@ -4177,15 +4171,6 @@
   </si>
   <si>
     <t>Composition.section:sectionDischargeNote</t>
-  </si>
-  <si>
-    <t>If not structured in sections (TBC)</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <t>Is the same section of the Admission Evaluation ? TBC</t>
   </si>
   <si>
     <t xml:space="preserve">equivalent				</t>
@@ -4280,6 +4265,9 @@
   </si>
   <si>
     <t>eHN Patient History Model to this guide Map</t>
+  </si>
+  <si>
+    <t>If not structured in sections</t>
   </si>
 </sst>
 </file>
@@ -4436,7 +4424,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4461,7 +4449,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5109,29 +5096,29 @@
     <col min="8" max="8" width="64.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5165,7 +5152,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$13</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>1179</v>
       </c>
       <c r="C3" s="9" t="str">
@@ -5190,7 +5177,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$13</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>1179</v>
       </c>
       <c r="C4" s="9" t="str">
@@ -5215,7 +5202,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$13</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>1327</v>
       </c>
       <c r="C5" s="9" t="str">
@@ -5240,7 +5227,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$13</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>1327</v>
       </c>
       <c r="C6" s="9" t="str">
@@ -5265,7 +5252,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$13</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/FunctionalStatus</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>1327</v>
       </c>
       <c r="C7" s="9" t="str">
@@ -5796,15 +5783,15 @@
         <f>LogicalModels!$A$15&amp;"."&amp;MedicationSummaryHdrEhn!A12</f>
         <v>MedicationSummary.daysSupplied</v>
       </c>
-      <c r="D14" s="35" t="str">
+      <c r="D14" s="34" t="str">
         <f>MedicationSummaryHdrEhn!D12</f>
         <v>A.2.9.2.11 - Days supplied</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>1135</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35" t="s">
+      <c r="F14" s="33"/>
+      <c r="G14" s="34" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="7"/>
@@ -5986,7 +5973,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>647</v>
@@ -6037,7 +6024,7 @@
         <v>66</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>650</v>
@@ -6106,7 +6093,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A2</f>
@@ -6123,7 +6110,7 @@
       <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="str">
@@ -6131,7 +6118,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A3</f>
@@ -6148,7 +6135,7 @@
       <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="str">
@@ -6156,7 +6143,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A4</f>
@@ -6180,7 +6167,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A5</f>
@@ -6204,7 +6191,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A6</f>
@@ -6228,7 +6215,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A7</f>
@@ -6252,7 +6239,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A8</f>
@@ -6276,7 +6263,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A9</f>
@@ -6300,7 +6287,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PlanOfCare</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1365</v>
+        <v>1360</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>LogicalModels!$A$14&amp;"."&amp;PlanOfCareHdrEhn!A10</f>
@@ -6441,7 +6428,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>635</v>
@@ -6458,7 +6445,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>636</v>
@@ -6509,7 +6496,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>639</v>
@@ -6603,7 +6590,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A2</f>
@@ -6621,7 +6608,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>1362</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
@@ -6630,7 +6617,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A3</f>
@@ -6655,7 +6642,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A4</f>
@@ -6680,7 +6667,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A5</f>
@@ -6690,8 +6677,8 @@
         <f>AdvanceDirectivesEhn!D5</f>
         <v>A.2.1.1.3 - Comment</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>1359</v>
+      <c r="E6" s="32" t="s">
+        <v>1354</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
@@ -6705,7 +6692,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A6</f>
@@ -6716,7 +6703,7 @@
         <v>A.2.1.1.4 - Related conditions</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>1360</v>
+        <v>1355</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
@@ -6730,7 +6717,7 @@
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdvanceDirectives</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1367</v>
+        <v>1362</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>LogicalModels!$A$5&amp;"."&amp;AdvanceDirectivesEhn!A7</f>
@@ -6827,7 +6814,7 @@
         <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>90</v>
@@ -6912,7 +6899,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>95</v>
@@ -7003,7 +6990,7 @@
         <v>1044</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A2</f>
@@ -7026,7 +7013,7 @@
         <v>1044</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A3</f>
@@ -7049,7 +7036,7 @@
         <v>1044</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A4</f>
@@ -7072,7 +7059,7 @@
         <v>1044</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A5</f>
@@ -7095,7 +7082,7 @@
         <v>1044</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A5</f>
@@ -7118,7 +7105,7 @@
         <v>1044</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A6</f>
@@ -7141,7 +7128,7 @@
         <v>1044</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A7</f>
@@ -7164,7 +7151,7 @@
         <v>1044</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A8</f>
@@ -7187,7 +7174,7 @@
         <v>1044</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A11</f>
@@ -7210,7 +7197,7 @@
         <v>1044</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A14</f>
@@ -7233,7 +7220,7 @@
         <v>1044</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A15</f>
@@ -7256,7 +7243,7 @@
         <v>1044</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>1368</v>
+        <v>1363</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A16</f>
@@ -7326,7 +7313,7 @@
         <v>1044</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A18</f>
@@ -7350,7 +7337,7 @@
         <v>1044</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>"Alerts."&amp;AlertsEhn!A18</f>
@@ -7426,7 +7413,7 @@
         <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>119</v>
@@ -7528,7 +7515,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>124</v>
@@ -7579,7 +7566,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>126</v>
@@ -7681,7 +7668,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>131</v>
@@ -7719,7 +7706,7 @@
   </sheetPr>
   <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -8221,7 +8208,7 @@
         <v>http://hl7.eu/fhir/hdr/ConceptMap/patientHistory2FHIR-eu-hdr</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1386</v>
+        <v>1381</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>1204</v>
@@ -8289,20 +8276,20 @@
     </row>
     <row r="14" spans="1:52" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="7" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.eu/fhir/hdr/ConceptMap/objectiveFindings2FHIR-eu-hdr</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>821</v>
@@ -8356,8 +8343,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8467,7 +8454,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>1363</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="88.5" x14ac:dyDescent="0.75">
@@ -8492,7 +8479,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="88.5" x14ac:dyDescent="0.75">
@@ -8694,7 +8681,7 @@
         <v>871</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C14" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A8</f>
@@ -8873,7 +8860,7 @@
         <v>871</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C22" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A15</f>
@@ -8898,7 +8885,7 @@
         <v>871</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C23" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A16</f>
@@ -8920,7 +8907,7 @@
         <v>871</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C24" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A17</f>
@@ -8945,7 +8932,7 @@
         <v>871</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C25" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A18</f>
@@ -8970,7 +8957,7 @@
         <v>871</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C26" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A19</f>
@@ -9039,7 +9026,7 @@
         <v>871</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C29" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A21</f>
@@ -9064,7 +9051,7 @@
         <v>871</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C30" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A22</f>
@@ -9086,7 +9073,7 @@
         <v>871</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C31" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A23</f>
@@ -9108,7 +9095,7 @@
         <v>871</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C32" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A24</f>
@@ -9130,7 +9117,7 @@
         <v>871</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C33" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A25</f>
@@ -9199,7 +9186,7 @@
         <v>871</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C36" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A27</f>
@@ -9224,7 +9211,7 @@
         <v>871</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C37" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A28</f>
@@ -9249,7 +9236,7 @@
         <v>871</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C38" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A29</f>
@@ -9274,7 +9261,7 @@
         <v>871</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C39" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A30</f>
@@ -9299,7 +9286,7 @@
         <v>871</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C40" t="str">
         <f>"Header"&amp;"."&amp;HeaderHdrEhn!A31</f>
@@ -9613,13 +9600,13 @@
         <f>HeaderHdrEhn!D42</f>
         <v>A.1.8.9 - Version</v>
       </c>
-      <c r="E53" s="34" t="s">
+      <c r="E53" s="33" t="s">
         <v>31</v>
       </c>
       <c r="G53" t="s">
         <v>33</v>
       </c>
-      <c r="H53" s="34" t="s">
+      <c r="H53" s="33" t="s">
         <v>35</v>
       </c>
     </row>
@@ -9732,7 +9719,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>851</v>
@@ -9800,7 +9787,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>713</v>
@@ -9868,7 +9855,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>717</v>
@@ -9936,7 +9923,7 @@
         <v>89</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>721</v>
@@ -10004,7 +9991,7 @@
         <v>66</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>725</v>
@@ -10038,7 +10025,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>727</v>
@@ -10106,7 +10093,7 @@
         <v>66</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>731</v>
@@ -10140,7 +10127,7 @@
         <v>64</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>733</v>
@@ -10208,7 +10195,7 @@
         <v>66</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>737</v>
@@ -10242,7 +10229,7 @@
         <v>66</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>739</v>
@@ -10344,7 +10331,7 @@
         <v>66</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>745</v>
@@ -11002,7 +10989,7 @@
         <v>945</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C15" t="str">
         <f>SubjectHdrEhn!A14</f>
@@ -11027,7 +11014,7 @@
         <v>945</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C16" t="str">
         <f>SubjectHdrEhn!A14</f>
@@ -11049,7 +11036,7 @@
         <v>945</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C17" t="str">
         <f>SubjectHdrEhn!A15</f>
@@ -11074,7 +11061,7 @@
         <v>945</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C18" t="str">
         <f>SubjectHdrEhn!A15</f>
@@ -11096,7 +11083,7 @@
         <v>945</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C19" t="str">
         <f>SubjectHdrEhn!A16</f>
@@ -11121,7 +11108,7 @@
         <v>945</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C20" t="str">
         <f>SubjectHdrEhn!A16</f>
@@ -11143,7 +11130,7 @@
         <v>945</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C21" t="str">
         <f>SubjectHdrEhn!A17</f>
@@ -11157,7 +11144,7 @@
         <v>985</v>
       </c>
       <c r="G21" t="s">
-        <v>1356</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
@@ -11165,7 +11152,7 @@
         <v>945</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C22" t="str">
         <f>SubjectHdrEhn!A18</f>
@@ -11187,7 +11174,7 @@
         <v>945</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C23" t="str">
         <f>SubjectHdrEhn!A19</f>
@@ -11212,7 +11199,7 @@
         <v>945</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C24" t="str">
         <f>SubjectHdrEhn!A19</f>
@@ -11234,7 +11221,7 @@
         <v>945</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C25" t="str">
         <f>SubjectHdrEhn!A20</f>
@@ -11259,7 +11246,7 @@
         <v>945</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C26" t="str">
         <f>SubjectHdrEhn!A20</f>
@@ -11540,7 +11527,7 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D2" t="s">
         <v>683</v>
@@ -11676,7 +11663,7 @@
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D10" t="s">
         <v>691</v>
@@ -11693,7 +11680,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" t="s">
         <v>692</v>
@@ -11744,7 +11731,7 @@
         <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D14" t="s">
         <v>695</v>
@@ -11812,7 +11799,7 @@
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D18" t="s">
         <v>699</v>
@@ -11863,7 +11850,7 @@
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D21" t="s">
         <v>702</v>
@@ -11982,7 +11969,7 @@
         <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D28" t="s">
         <v>709</v>
@@ -12050,26 +12037,26 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$8</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdmissionEvaluation</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>862</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>LogicalModels!$A$8&amp;"."&amp;AdmissionEvaluationEhn!A2</f>
         <v>AdmissionEvaluation.objectiveFindings</v>
       </c>
-      <c r="D2" s="35" t="str">
+      <c r="D2" s="34" t="str">
         <f>AdmissionEvaluationEhn!D2</f>
         <v>A.2.4.1 - Objective findings</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>1152</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35" t="s">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="36" t="s">
-        <v>1358</v>
+      <c r="H2" s="35" t="s">
+        <v>1353</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
@@ -12077,25 +12064,25 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$8</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/AdmissionEvaluation</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>862</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>LogicalModels!$A$8&amp;"."&amp;AdmissionEvaluationEhn!A3</f>
         <v>AdmissionEvaluation.functionalStatus</v>
       </c>
-      <c r="D3" s="35" t="str">
+      <c r="D3" s="34" t="str">
         <f>AdmissionEvaluationEhn!D3</f>
         <v>A.2.4.2 - Functional status</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>1183</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="34"/>
+      <c r="G3" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="35" t="s">
         <v>1322</v>
       </c>
     </row>
@@ -12367,7 +12354,7 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>1369</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
@@ -12375,7 +12362,7 @@
         <v>860</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C8" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A8</f>
@@ -12392,7 +12379,7 @@
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>1370</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
@@ -12400,7 +12387,7 @@
         <v>860</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C9" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A8</f>
@@ -12417,7 +12404,7 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>1371</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -12425,7 +12412,7 @@
         <v>860</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C10" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A9</f>
@@ -12467,7 +12454,7 @@
         <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>1372</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
@@ -12514,7 +12501,7 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>1373</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
@@ -12569,7 +12556,7 @@
         <v>860</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C16" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A14</f>
@@ -12586,7 +12573,7 @@
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>1374</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
@@ -12594,7 +12581,7 @@
         <v>860</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="C17" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A14</f>
@@ -12611,7 +12598,7 @@
         <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>1375</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -12619,7 +12606,7 @@
         <v>860</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="C18" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A15</f>
@@ -12661,7 +12648,7 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>1376</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
@@ -12686,7 +12673,7 @@
         <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>1377</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
@@ -12788,12 +12775,12 @@
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A21</f>
         <v>Encounter.admissionReason.legalStatus</v>
       </c>
-      <c r="D25" s="32" t="str">
+      <c r="D25" s="31" t="str">
         <f>EncounterEhn!D21</f>
         <v>A.2.3.4.3 - Admission legal status</v>
       </c>
       <c r="E25" t="s">
-        <v>1361</v>
+        <v>1356</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
@@ -12914,7 +12901,7 @@
         <v>860</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
       <c r="C31" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A27</f>
@@ -12925,7 +12912,7 @@
         <v>A.2.3.6.1 - Period</v>
       </c>
       <c r="E31" t="s">
-        <v>1357</v>
+        <v>1352</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
@@ -12939,7 +12926,7 @@
         <v>860</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
       <c r="C32" t="str">
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A28</f>
@@ -13020,17 +13007,17 @@
         <f>"Encounter"&amp;"."&amp;EncounterEhn!A31</f>
         <v>Encounter.location.organization.details</v>
       </c>
-      <c r="D35" s="34" t="str">
+      <c r="D35" s="33" t="str">
         <f>EncounterEhn!D31</f>
         <v>A.2.3.6.4 - Organisation Part Details</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="33" t="s">
         <v>228</v>
       </c>
       <c r="G35" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="34" t="s">
+      <c r="H35" s="33" t="s">
         <v>15</v>
       </c>
     </row>
@@ -13150,7 +13137,7 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D4" t="s">
         <v>204</v>
@@ -13201,7 +13188,7 @@
         <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D7" t="s">
         <v>207</v>
@@ -13269,7 +13256,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" t="s">
         <v>211</v>
@@ -13303,7 +13290,7 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D13" t="s">
         <v>213</v>
@@ -13371,7 +13358,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D17" t="s">
         <v>217</v>
@@ -13388,7 +13375,7 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D18" t="s">
         <v>218</v>
@@ -13456,7 +13443,7 @@
         <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D22" t="s">
         <v>222</v>
@@ -13524,7 +13511,7 @@
         <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D26" t="s">
         <v>226</v>
@@ -13558,7 +13545,7 @@
         <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D28" t="s">
         <v>228</v>
@@ -13609,7 +13596,7 @@
         <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D31" t="s">
         <v>231</v>
@@ -13630,8 +13617,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -13677,7 +13664,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C2" s="7" t="str">
@@ -13695,14 +13682,14 @@
       <c r="G2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>862</v>
       </c>
       <c r="C3" s="7" t="str">
@@ -13720,17 +13707,15 @@
       <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>1337</v>
-      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>1341</v>
+      <c r="B4" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A4</f>
@@ -13747,17 +13732,15 @@
       <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>1341</v>
+      <c r="B5" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A5</f>
@@ -13774,17 +13757,15 @@
       <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>1341</v>
+      <c r="B6" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A6</f>
@@ -13801,16 +13782,14 @@
       <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>862</v>
       </c>
       <c r="C7" s="7" t="str">
@@ -13822,21 +13801,21 @@
         <v>A.2.8.1.4 - Vital signs</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>1341</v>
+      <c r="B8" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A8</f>
@@ -13853,17 +13832,15 @@
       <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>1341</v>
+      <c r="B9" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A9</f>
@@ -13880,17 +13857,15 @@
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>1341</v>
+      <c r="B10" s="22" t="s">
+        <v>1340</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>LogicalModels!$A$12&amp;"."&amp;ObjectiveFindingsHdrEhn!A10</f>
@@ -13907,16 +13882,14 @@
       <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>1342</v>
-      </c>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="7" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>862</v>
       </c>
       <c r="C11" s="7" t="str">
@@ -13928,7 +13901,7 @@
         <v>A.2.8.1.5 - Physical examination</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
@@ -13941,7 +13914,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$12</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/ObjectiveFindings</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>862</v>
       </c>
       <c r="C12" s="7" t="str">
@@ -13953,7 +13926,7 @@
         <v>A.2.8.1.5.1 - Observation Note</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
@@ -14031,7 +14004,7 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D3" t="s">
         <v>149</v>
@@ -14065,7 +14038,7 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D5" t="s">
         <v>151</v>
@@ -14082,7 +14055,7 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D6" t="s">
         <v>152</v>
@@ -14099,7 +14072,7 @@
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D7" t="s">
         <v>153</v>
@@ -14133,7 +14106,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D9" t="s">
         <v>155</v>
@@ -14150,7 +14123,7 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D10" t="s">
         <v>156</v>
@@ -14167,7 +14140,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" t="s">
         <v>157</v>
@@ -14472,29 +14445,29 @@
     <col min="8" max="8" width="93.6796875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -14987,7 +14960,7 @@
         <v>1230</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="9"/>
@@ -15012,7 +14985,7 @@
         <v>1234</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="9" t="s">
@@ -15219,7 +15192,7 @@
       <c r="G29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H29" s="21"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="8" t="str">
@@ -15244,7 +15217,7 @@
       <c r="G30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="21"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="str">
@@ -15301,7 +15274,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="23" t="s">
         <v>862</v>
       </c>
       <c r="C33" s="9" t="str">
@@ -15326,7 +15299,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C34" s="9" t="str">
@@ -15350,7 +15323,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C35" s="9" t="str">
@@ -15375,7 +15348,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C36" s="9" t="str">
@@ -15400,7 +15373,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C37" s="9" t="str">
@@ -15425,7 +15398,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C38" s="9" t="str">
@@ -15450,7 +15423,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>1291</v>
       </c>
       <c r="C39" s="9" t="str">
@@ -15465,7 +15438,7 @@
         <v>1283</v>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H39" s="9"/>
@@ -15475,8 +15448,8 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B40" s="24" t="s">
-        <v>1385</v>
+      <c r="B40" s="23" t="s">
+        <v>1380</v>
       </c>
       <c r="C40" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A33</f>
@@ -15490,7 +15463,7 @@
         <v>1285</v>
       </c>
       <c r="F40" s="7"/>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="19" t="s">
         <v>20</v>
       </c>
       <c r="H40" s="9"/>
@@ -15500,7 +15473,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="22" t="s">
         <v>862</v>
       </c>
       <c r="C41" s="9" t="str">
@@ -15515,11 +15488,11 @@
         <v>1152</v>
       </c>
       <c r="F41" s="7"/>
-      <c r="G41" s="38" t="s">
+      <c r="G41" s="37" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>1366</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.75">
@@ -15527,7 +15500,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="23" t="s">
         <v>862</v>
       </c>
       <c r="C42" s="9" t="str">
@@ -15552,7 +15525,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="C43" s="9" t="str">
@@ -15577,7 +15550,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="C44" s="9" t="str">
@@ -15604,7 +15577,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="C45" s="9" t="str">
@@ -15631,7 +15604,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="C46" s="9" t="str">
@@ -15658,7 +15631,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="23" t="s">
         <v>1315</v>
       </c>
       <c r="C47" s="9" t="str">
@@ -15683,7 +15656,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="23" t="s">
         <v>862</v>
       </c>
       <c r="C48" s="9" t="str">
@@ -15708,7 +15681,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="23" t="s">
         <v>1319</v>
       </c>
       <c r="C49" s="9" t="str">
@@ -15733,7 +15706,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="23" t="s">
         <v>1319</v>
       </c>
       <c r="C50" s="9" t="str">
@@ -15758,7 +15731,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="23" t="s">
         <v>1319</v>
       </c>
       <c r="C51" s="9" t="str">
@@ -15783,7 +15756,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="26" t="s">
         <v>862</v>
       </c>
       <c r="C52" s="9" t="str">
@@ -15794,22 +15767,22 @@
         <f xml:space="preserve"> PatientHistoryEhn!D45</f>
         <v>A.2.6.2 - Family history</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="E52" s="24" t="s">
         <v>1301</v>
       </c>
       <c r="F52" s="7"/>
-      <c r="G52" s="26" t="s">
+      <c r="G52" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="25"/>
+      <c r="H52" s="24"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A53" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B53" s="24" t="s">
-        <v>1378</v>
+      <c r="B53" s="23" t="s">
+        <v>1373</v>
       </c>
       <c r="C53" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A46</f>
@@ -15819,22 +15792,22 @@
         <f xml:space="preserve"> PatientHistoryEhn!D46</f>
         <v>A.2.6.2.1 - Patient relationship</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="15" t="s">
         <v>1302</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H53" s="25"/>
+      <c r="H53" s="24"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A54" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B54" s="24" t="s">
-        <v>1378</v>
+      <c r="B54" s="23" t="s">
+        <v>1373</v>
       </c>
       <c r="C54" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A47</f>
@@ -15844,22 +15817,22 @@
         <f xml:space="preserve"> PatientHistoryEhn!D47</f>
         <v>A.2.6.2.2 - Date of birth</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="15" t="s">
         <v>1303</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="25"/>
+      <c r="H54" s="24"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A55" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B55" s="24" t="s">
-        <v>1378</v>
+      <c r="B55" s="23" t="s">
+        <v>1373</v>
       </c>
       <c r="C55" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A48</f>
@@ -15869,22 +15842,22 @@
         <f xml:space="preserve"> PatientHistoryEhn!D48</f>
         <v>A.2.6.2.3 - Age or date of death</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="15" t="s">
         <v>1304</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H55" s="25"/>
+      <c r="H55" s="24"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A56" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B56" s="24" t="s">
-        <v>1378</v>
+      <c r="B56" s="23" t="s">
+        <v>1373</v>
       </c>
       <c r="C56" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A49</f>
@@ -15894,22 +15867,22 @@
         <f xml:space="preserve"> PatientHistoryEhn!D49</f>
         <v>A.2.6.2.5 - Condition</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>1305</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H56" s="25"/>
+      <c r="H56" s="24"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A57" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B57" s="24" t="s">
-        <v>1378</v>
+      <c r="B57" s="23" t="s">
+        <v>1373</v>
       </c>
       <c r="C57" s="9" t="str">
         <f>LogicalModels!$A$9&amp;"."&amp;PatientHistoryEhn!A50</f>
@@ -15919,14 +15892,14 @@
         <f xml:space="preserve"> PatientHistoryEhn!D50</f>
         <v>A.2.6.2.6 - Cause of death</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>1305</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H57" s="25" t="s">
+      <c r="H57" s="24" t="s">
         <v>1306</v>
       </c>
     </row>
@@ -15935,7 +15908,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="26" t="s">
         <v>862</v>
       </c>
       <c r="C58" s="9" t="str">
@@ -15946,21 +15919,21 @@
         <f xml:space="preserve"> PatientHistoryEhn!D51</f>
         <v>A.2.6.3 - Social determinants of health</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="E58" s="24" t="s">
         <v>1288</v>
       </c>
       <c r="F58" s="7"/>
-      <c r="G58" s="26" t="s">
+      <c r="G58" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H58" s="25"/>
+      <c r="H58" s="24"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A59" s="8" t="str">
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C59" s="9" t="str">
@@ -15987,7 +15960,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C60" s="9" t="str">
@@ -16014,7 +15987,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C61" s="9" t="str">
@@ -16041,7 +16014,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C62" s="9" t="str">
@@ -16068,7 +16041,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C63" s="9" t="str">
@@ -16095,7 +16068,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C64" s="9" t="str">
@@ -16122,7 +16095,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C65" s="9" t="str">
@@ -16149,7 +16122,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B66" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C66" s="9" t="str">
@@ -16176,7 +16149,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B67" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C67" s="9" t="str">
@@ -16203,7 +16176,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C68" s="9" t="str">
@@ -16230,7 +16203,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C69" s="9" t="str">
@@ -16257,7 +16230,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C70" s="9" t="str">
@@ -16284,7 +16257,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C71" s="9" t="str">
@@ -16311,7 +16284,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B72" s="24" t="s">
+      <c r="B72" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C72" s="9" t="str">
@@ -16338,7 +16311,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B73" s="24" t="s">
+      <c r="B73" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C73" s="9" t="str">
@@ -16365,7 +16338,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B74" s="24" t="s">
+      <c r="B74" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C74" s="9" t="str">
@@ -16392,7 +16365,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C75" s="9" t="str">
@@ -16419,7 +16392,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B76" s="24" t="s">
+      <c r="B76" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C76" s="9" t="str">
@@ -16446,7 +16419,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B77" s="24" t="s">
+      <c r="B77" s="23" t="s">
         <v>1307</v>
       </c>
       <c r="C77" s="9" t="str">
@@ -16473,7 +16446,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B78" s="23" t="s">
+      <c r="B78" s="22" t="s">
         <v>862</v>
       </c>
       <c r="C78" s="9" t="str">
@@ -16500,7 +16473,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C79" s="9" t="str">
@@ -16527,7 +16500,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C80" s="9" t="str">
@@ -16554,7 +16527,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B81" s="23" t="s">
+      <c r="B81" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C81" s="9" t="str">
@@ -16581,7 +16554,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B82" s="23" t="s">
+      <c r="B82" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C82" s="9" t="str">
@@ -16608,7 +16581,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C83" s="9" t="str">
@@ -16635,7 +16608,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B84" s="23" t="s">
+      <c r="B84" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C84" s="9" t="str">
@@ -16662,7 +16635,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B85" s="23" t="s">
+      <c r="B85" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C85" s="9" t="str">
@@ -16689,7 +16662,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C86" s="9" t="str">
@@ -16716,7 +16689,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B87" s="23" t="s">
+      <c r="B87" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C87" s="9" t="str">
@@ -16743,7 +16716,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B88" s="23" t="s">
+      <c r="B88" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C88" s="9" t="str">
@@ -16770,7 +16743,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B89" s="23" t="s">
+      <c r="B89" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C89" s="9" t="str">
@@ -16797,7 +16770,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B90" s="23" t="s">
+      <c r="B90" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C90" s="9" t="str">
@@ -16824,7 +16797,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B91" s="23" t="s">
+      <c r="B91" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C91" s="9" t="str">
@@ -16851,7 +16824,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$9</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/PatientHistory</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="B92" s="22" t="s">
         <v>1311</v>
       </c>
       <c r="C92" s="9" t="str">
@@ -16884,7 +16857,7 @@
       <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="C95" s="28"/>
+      <c r="C95" s="27"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
@@ -16969,7 +16942,7 @@
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D2" t="s">
         <v>480</v>
@@ -16986,7 +16959,7 @@
         <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D3" t="s">
         <v>481</v>
@@ -17020,7 +16993,7 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D5" t="s">
         <v>483</v>
@@ -17088,7 +17061,7 @@
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D9" t="s">
         <v>487</v>
@@ -17139,7 +17112,7 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D12" t="s">
         <v>490</v>
@@ -17241,7 +17214,7 @@
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D18" t="s">
         <v>496</v>
@@ -17360,7 +17333,7 @@
         <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D25" t="s">
         <v>503</v>
@@ -17377,7 +17350,7 @@
         <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D26" t="s">
         <v>504</v>
@@ -17445,7 +17418,7 @@
         <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D30" t="s">
         <v>853</v>
@@ -17513,7 +17486,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D34" t="s">
         <v>511</v>
@@ -17530,7 +17503,7 @@
         <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D35" t="s">
         <v>512</v>
@@ -17632,7 +17605,7 @@
         <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D41" t="s">
         <v>518</v>
@@ -17700,7 +17673,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D45" t="s">
         <v>522</v>
@@ -17751,7 +17724,7 @@
         <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D48" t="s">
         <v>525</v>
@@ -17768,7 +17741,7 @@
         <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D49" t="s">
         <v>526</v>
@@ -17802,7 +17775,7 @@
         <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D51" t="s">
         <v>528</v>
@@ -17819,7 +17792,7 @@
         <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D52" t="s">
         <v>529</v>
@@ -17887,7 +17860,7 @@
         <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D56" t="s">
         <v>533</v>
@@ -17938,7 +17911,7 @@
         <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D59" t="s">
         <v>536</v>
@@ -18006,7 +17979,7 @@
         <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D63" t="s">
         <v>540</v>
@@ -18108,7 +18081,7 @@
         <v>65</v>
       </c>
       <c r="C69" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D69" t="s">
         <v>546</v>
@@ -18125,7 +18098,7 @@
         <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D70" t="s">
         <v>547</v>
@@ -18142,7 +18115,7 @@
         <v>64</v>
       </c>
       <c r="C71" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D71" t="s">
         <v>548</v>
@@ -18159,7 +18132,7 @@
         <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D72" t="s">
         <v>549</v>
@@ -18227,7 +18200,7 @@
         <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D76" t="s">
         <v>553</v>
@@ -18261,7 +18234,7 @@
         <v>65</v>
       </c>
       <c r="C78" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D78" t="s">
         <v>555</v>
@@ -18295,7 +18268,7 @@
         <v>65</v>
       </c>
       <c r="C80" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D80" t="s">
         <v>557</v>
@@ -18329,7 +18302,7 @@
         <v>64</v>
       </c>
       <c r="C82" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D82" t="s">
         <v>559</v>
@@ -18401,7 +18374,7 @@
   </sheetPr>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="C42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -18417,29 +18390,29 @@
     <col min="8" max="8" width="64.7265625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -19022,7 +18995,7 @@
       <c r="G24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="8" t="str">
@@ -19196,7 +19169,7 @@
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A25</f>
         <v>HospitalStay.medicalDevices.implantDate</v>
       </c>
-      <c r="D31" s="37" t="str">
+      <c r="D31" s="36" t="str">
         <f xml:space="preserve"> HospitalStayEhn!D25</f>
         <v>A.2.7.3.3 - Implant date</v>
       </c>
@@ -19223,7 +19196,7 @@
         <f>LogicalModels!$A$10&amp;"."&amp;HospitalStayEhn!A25</f>
         <v>HospitalStay.medicalDevices.implantDate</v>
       </c>
-      <c r="D32" s="37" t="str">
+      <c r="D32" s="36" t="str">
         <f xml:space="preserve"> HospitalStayEhn!D25</f>
         <v>A.2.7.3.3 - Implant date</v>
       </c>
@@ -19258,10 +19231,10 @@
         <v>1230</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="21"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="8" t="str">
@@ -19283,10 +19256,10 @@
         <v>1234</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="21"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A35" s="8" t="str">
@@ -19345,7 +19318,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="22" t="s">
         <v>1250</v>
       </c>
       <c r="C37" s="9" t="str">
@@ -19370,7 +19343,7 @@
         <f>"http://hl7.eu/fhir/hdr/StructureDefinition/"&amp;LogicalModels!$A$10</f>
         <v>http://hl7.eu/fhir/hdr/StructureDefinition/HospitalStay</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>1250</v>
       </c>
       <c r="C38" s="9" t="str">
@@ -19840,7 +19813,7 @@
       <c r="G56" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="22" t="s">
+      <c r="H56" s="21" t="s">
         <v>1246</v>
       </c>
     </row>
@@ -20487,7 +20460,7 @@
         <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D2" t="s">
         <v>306</v>
@@ -20521,7 +20494,7 @@
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D4" t="s">
         <v>308</v>
@@ -20623,7 +20596,7 @@
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D10" t="s">
         <v>314</v>
@@ -20674,7 +20647,7 @@
         <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D13" t="s">
         <v>317</v>
@@ -20810,7 +20783,7 @@
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D21" t="s">
         <v>325</v>
@@ -20827,7 +20800,7 @@
         <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D22" t="s">
         <v>326</v>
@@ -20929,7 +20902,7 @@
         <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D28" t="s">
         <v>332</v>
@@ -21065,7 +21038,7 @@
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D36" t="s">
         <v>340</v>
@@ -21116,7 +21089,7 @@
         <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D39" t="s">
         <v>343</v>
@@ -21184,7 +21157,7 @@
         <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D43" t="s">
         <v>347</v>
@@ -21201,7 +21174,7 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D44" t="s">
         <v>348</v>
@@ -21218,7 +21191,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D45" t="s">
         <v>349</v>
@@ -21235,7 +21208,7 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D46" t="s">
         <v>350</v>
@@ -21291,7 +21264,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H12" sqref="H12:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -21306,29 +21279,29 @@
     <col min="8" max="8" width="64.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -21403,7 +21376,7 @@
         <v>A.2.0 - Hospital Discharge Report in its narrative form</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>1364</v>
+        <v>1359</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
@@ -21434,7 +21407,7 @@
       <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="26"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="str">
@@ -21460,7 +21433,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
@@ -21514,7 +21487,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
@@ -21541,7 +21514,7 @@
         <v>20</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
@@ -21568,7 +21541,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
@@ -21595,7 +21568,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -21614,7 +21587,7 @@
         <f>HospitalDischargeReportEhn!D12</f>
         <v>A.2.7.1 - Objective findings</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>1139</v>
       </c>
       <c r="F12" s="7"/>
@@ -21622,7 +21595,7 @@
         <v>20</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>1353</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -21641,16 +21614,14 @@
         <f>HospitalDischargeReportEhn!D12</f>
         <v>A.2.7.1 - Objective findings</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="29" t="s">
         <v>1182</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>1354</v>
-      </c>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="8" t="str">
@@ -21668,7 +21639,7 @@
         <f>HospitalDischargeReportEhn!D13</f>
         <v>A.2.7.2 - Functional status</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="29" t="s">
         <v>1139</v>
       </c>
       <c r="F14" s="7"/>
@@ -21676,7 +21647,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>1353</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -21695,16 +21666,14 @@
         <f>HospitalDischargeReportEhn!D13</f>
         <v>A.2.7.2 - Functional status</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>1183</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>1355</v>
-      </c>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="8"/>
@@ -21717,15 +21686,12 @@
         <f>HospitalDischargeReportEhn!D14</f>
         <v>A.2.7.3 - Discharge note</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>1352</v>
+      <c r="E16" s="29" t="s">
+        <v>1350</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
@@ -21744,7 +21710,7 @@
         <f>HospitalDischargeReportEhn!D14</f>
         <v>A.2.7.3 - Discharge note</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="29" t="s">
         <v>1184</v>
       </c>
       <c r="F17" s="7"/>
@@ -21752,7 +21718,7 @@
         <v>20</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>1354</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
@@ -21936,7 +21902,7 @@
         <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D3" t="s">
         <v>749</v>
@@ -21953,7 +21919,7 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D4" t="s">
         <v>750</v>
@@ -22072,7 +22038,7 @@
         <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D11" t="s">
         <v>879</v>
@@ -22142,7 +22108,7 @@
         <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="D15" t="s">
         <v>880</v>

</xml_diff>